<commit_message>
updated template for report
git-svn-id: svn://107.170.10.188:8080/Semoss/trunk@2871 ef391c1c-ee15-45f7-b1d6-dde3d27a2169

Former-commit-id: 6e140540f2907a5302d62fbe5087880aaaba0949
</commit_message>
<xml_diff>
--- a/export/Reports/TAP_Legacy_System_Dispositions_Template.xlsx
+++ b/export/Reports/TAP_Legacy_System_Dispositions_Template.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mahkhalil\workspace\Semoss\export\Reports\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="480" yWindow="255" windowWidth="22995" windowHeight="8580"/>
   </bookViews>
@@ -10,12 +15,12 @@
     <sheet name="Disposition Overview" sheetId="1" r:id="rId1"/>
     <sheet name="Summary Charts" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="152511" calcOnSave="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="50">
   <si>
     <t>ABACUS</t>
   </si>
@@ -32,12 +37,6 @@
     <t>Description</t>
   </si>
   <si>
-    <t>Low Probability with Integration (LPI)</t>
-  </si>
-  <si>
-    <t>LPI systems were designated by the Functional Advisory Council (FAC) as having a low probability of being replaced by the DHMSM EHR solution and were also designated as requiring integration with DHMSM in order to support data exchange.</t>
-  </si>
-  <si>
     <t>Modernization Activities</t>
   </si>
   <si>
@@ -69,9 +68,6 @@
   </si>
   <si>
     <t>System Owner</t>
-  </si>
-  <si>
-    <t>Army</t>
   </si>
   <si>
     <t>ATO Date</t>
@@ -159,13 +155,22 @@
     <t>Proposed Future Interfaces with DHMSM - Legacy Consumer</t>
   </si>
   <si>
-    <t>REQUIRES IMMEDIATE ACCREDITATION</t>
-  </si>
-  <si>
     <t>**Interface Modernization activities involve upgrading the legacy system to be able to exchange data with COTS EHR solution via SOA services. It is assumed that these activities must be completed before the COTS EHR solution is fielded.</t>
   </si>
   <si>
     <t>Interface Modernization**</t>
+  </si>
+  <si>
+    <t>SysName</t>
+  </si>
+  <si>
+    <t>SysOwner</t>
+  </si>
+  <si>
+    <t>Sys Category</t>
+  </si>
+  <si>
+    <t>Sys Category Description</t>
   </si>
 </sst>
 </file>
@@ -337,7 +342,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="46">
+  <borders count="45">
     <border>
       <left/>
       <right/>
@@ -788,17 +793,6 @@
         <color indexed="64"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
         <color indexed="64"/>
       </right>
       <top/>
@@ -928,7 +922,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="112">
+  <cellXfs count="111">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="44" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -938,9 +932,6 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="8" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -957,6 +948,264 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="2" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="8" fillId="7" borderId="38" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="8" fillId="7" borderId="39" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="8" fillId="7" borderId="35" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="8" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="8" fillId="0" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="8" fillId="0" borderId="37" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="8" fillId="0" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="7" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="7" fillId="0" borderId="14" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="7" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="7" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -979,264 +1228,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="7" fillId="0" borderId="20" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="7" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="7" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="7" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="7" fillId="0" borderId="14" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="8" fillId="0" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="8" fillId="7" borderId="35" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="8" fillId="7" borderId="36" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="8" fillId="7" borderId="39" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="8" fillId="7" borderId="40" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="8" fillId="0" borderId="38" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="8" fillId="0" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="5" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1250,6 +1241,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1453,11 +1447,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="154754048"/>
-        <c:axId val="154759936"/>
+        <c:axId val="535397864"/>
+        <c:axId val="535398256"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="154754048"/>
+        <c:axId val="535397864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1466,7 +1460,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="154759936"/>
+        <c:crossAx val="535398256"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1474,7 +1468,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="154759936"/>
+        <c:axId val="535398256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1485,7 +1479,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="154754048"/>
+        <c:crossAx val="535397864"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1659,7 +1653,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1694,7 +1688,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1905,8 +1899,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:N37"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K6" sqref="K6:N6"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I28" sqref="I28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1922,607 +1916,631 @@
   <sheetData>
     <row r="1" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:14" ht="72" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="64" t="s">
-        <v>34</v>
-      </c>
-      <c r="C2" s="65"/>
-      <c r="D2" s="66" t="s">
-        <v>35</v>
-      </c>
-      <c r="E2" s="67"/>
-      <c r="F2" s="67"/>
-      <c r="G2" s="67"/>
-      <c r="H2" s="67"/>
-      <c r="I2" s="67"/>
-      <c r="J2" s="67"/>
-      <c r="K2" s="67"/>
-      <c r="L2" s="67"/>
-      <c r="M2" s="79"/>
-      <c r="N2" s="68"/>
+      <c r="B2" s="46" t="s">
+        <v>31</v>
+      </c>
+      <c r="C2" s="47"/>
+      <c r="D2" s="48" t="s">
+        <v>32</v>
+      </c>
+      <c r="E2" s="49"/>
+      <c r="F2" s="49"/>
+      <c r="G2" s="49"/>
+      <c r="H2" s="49"/>
+      <c r="I2" s="49"/>
+      <c r="J2" s="49"/>
+      <c r="K2" s="49"/>
+      <c r="L2" s="49"/>
+      <c r="M2" s="50"/>
+      <c r="N2" s="51"/>
     </row>
     <row r="3" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="4" spans="2:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="26" t="s">
-        <v>0</v>
-      </c>
-      <c r="C4" s="27"/>
-      <c r="D4" s="28" t="s">
+    <row r="4" spans="2:14" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="79" t="s">
+        <v>46</v>
+      </c>
+      <c r="C4" s="80"/>
+      <c r="D4" s="81" t="s">
         <v>1</v>
       </c>
-      <c r="E4" s="28"/>
-      <c r="F4" s="28"/>
-      <c r="G4" s="28"/>
-      <c r="H4" s="28"/>
-      <c r="I4" s="28"/>
-      <c r="J4" s="28"/>
-      <c r="K4" s="28"/>
-      <c r="L4" s="28"/>
-      <c r="M4" s="80"/>
-      <c r="N4" s="29"/>
+      <c r="E4" s="81"/>
+      <c r="F4" s="81"/>
+      <c r="G4" s="81"/>
+      <c r="H4" s="81"/>
+      <c r="I4" s="81"/>
+      <c r="J4" s="81"/>
+      <c r="K4" s="81"/>
+      <c r="L4" s="81"/>
+      <c r="M4" s="82"/>
+      <c r="N4" s="83"/>
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B5" s="69" t="s">
-        <v>17</v>
-      </c>
-      <c r="C5" s="70"/>
-      <c r="D5" s="71" t="s">
-        <v>18</v>
-      </c>
-      <c r="E5" s="71"/>
-      <c r="F5" s="71"/>
-      <c r="G5" s="71"/>
-      <c r="H5" s="71"/>
-      <c r="I5" s="71"/>
-      <c r="J5" s="71"/>
-      <c r="K5" s="71"/>
-      <c r="L5" s="71"/>
-      <c r="M5" s="81"/>
-      <c r="N5" s="72"/>
+      <c r="B5" s="52" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="53"/>
+      <c r="D5" s="54" t="s">
+        <v>47</v>
+      </c>
+      <c r="E5" s="54"/>
+      <c r="F5" s="54"/>
+      <c r="G5" s="54"/>
+      <c r="H5" s="54"/>
+      <c r="I5" s="54"/>
+      <c r="J5" s="54"/>
+      <c r="K5" s="54"/>
+      <c r="L5" s="54"/>
+      <c r="M5" s="55"/>
+      <c r="N5" s="56"/>
     </row>
     <row r="6" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="30" t="s">
-        <v>19</v>
-      </c>
-      <c r="C6" s="31"/>
-      <c r="D6" s="42" t="s">
-        <v>20</v>
-      </c>
-      <c r="E6" s="42"/>
-      <c r="F6" s="42"/>
-      <c r="G6" s="42"/>
-      <c r="H6" s="42"/>
-      <c r="I6" s="41" t="s">
-        <v>43</v>
-      </c>
-      <c r="J6" s="41"/>
-      <c r="K6" s="108" t="s">
-        <v>47</v>
-      </c>
-      <c r="L6" s="109"/>
-      <c r="M6" s="110"/>
-      <c r="N6" s="111"/>
+      <c r="B6" s="84" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" s="85"/>
+      <c r="D6" s="102">
+        <v>42005</v>
+      </c>
+      <c r="E6" s="102"/>
+      <c r="F6" s="102"/>
+      <c r="G6" s="102"/>
+      <c r="H6" s="102"/>
+      <c r="I6" s="97" t="s">
+        <v>40</v>
+      </c>
+      <c r="J6" s="97"/>
+      <c r="K6" s="98">
+        <v>42005</v>
+      </c>
+      <c r="L6" s="99"/>
+      <c r="M6" s="100"/>
+      <c r="N6" s="101"/>
     </row>
     <row r="7" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="8" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B8" s="32" t="s">
+      <c r="B8" s="86" t="s">
         <v>3</v>
       </c>
-      <c r="C8" s="33"/>
-      <c r="D8" s="36" t="s">
+      <c r="C8" s="87"/>
+      <c r="D8" s="90" t="s">
         <v>2</v>
       </c>
-      <c r="E8" s="36"/>
-      <c r="F8" s="36"/>
-      <c r="G8" s="36" t="s">
+      <c r="E8" s="90"/>
+      <c r="F8" s="90"/>
+      <c r="G8" s="90" t="s">
         <v>4</v>
       </c>
-      <c r="H8" s="36"/>
-      <c r="I8" s="36"/>
-      <c r="J8" s="36"/>
-      <c r="K8" s="36"/>
-      <c r="L8" s="36"/>
-      <c r="M8" s="82"/>
-      <c r="N8" s="37"/>
+      <c r="H8" s="90"/>
+      <c r="I8" s="90"/>
+      <c r="J8" s="90"/>
+      <c r="K8" s="90"/>
+      <c r="L8" s="90"/>
+      <c r="M8" s="91"/>
+      <c r="N8" s="92"/>
     </row>
     <row r="9" spans="2:14" ht="40.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="34"/>
-      <c r="C9" s="35"/>
-      <c r="D9" s="38" t="s">
-        <v>5</v>
-      </c>
-      <c r="E9" s="38"/>
-      <c r="F9" s="38"/>
-      <c r="G9" s="39" t="s">
-        <v>6</v>
-      </c>
-      <c r="H9" s="39"/>
-      <c r="I9" s="39"/>
-      <c r="J9" s="39"/>
-      <c r="K9" s="39"/>
-      <c r="L9" s="39"/>
-      <c r="M9" s="83"/>
-      <c r="N9" s="40"/>
+      <c r="B9" s="88"/>
+      <c r="C9" s="89"/>
+      <c r="D9" s="93" t="s">
+        <v>48</v>
+      </c>
+      <c r="E9" s="93"/>
+      <c r="F9" s="93"/>
+      <c r="G9" s="94" t="s">
+        <v>49</v>
+      </c>
+      <c r="H9" s="94"/>
+      <c r="I9" s="94"/>
+      <c r="J9" s="94"/>
+      <c r="K9" s="94"/>
+      <c r="L9" s="94"/>
+      <c r="M9" s="95"/>
+      <c r="N9" s="96"/>
     </row>
     <row r="10" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="11" spans="2:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="52" t="s">
-        <v>21</v>
-      </c>
-      <c r="C11" s="53"/>
-      <c r="D11" s="53"/>
-      <c r="E11" s="53"/>
-      <c r="F11" s="53"/>
-      <c r="G11" s="53"/>
-      <c r="H11" s="53"/>
-      <c r="I11" s="53"/>
-      <c r="J11" s="53"/>
-      <c r="K11" s="53"/>
-      <c r="L11" s="53"/>
-      <c r="M11" s="84"/>
-      <c r="N11" s="54"/>
+      <c r="B11" s="31" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" s="32"/>
+      <c r="D11" s="32"/>
+      <c r="E11" s="32"/>
+      <c r="F11" s="32"/>
+      <c r="G11" s="32"/>
+      <c r="H11" s="32"/>
+      <c r="I11" s="32"/>
+      <c r="J11" s="32"/>
+      <c r="K11" s="32"/>
+      <c r="L11" s="32"/>
+      <c r="M11" s="33"/>
+      <c r="N11" s="34"/>
     </row>
     <row r="12" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="13" spans="2:14" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="48" t="s">
+      <c r="B13" s="75" t="s">
+        <v>5</v>
+      </c>
+      <c r="C13" s="76"/>
+      <c r="D13" s="76"/>
+      <c r="E13" s="76"/>
+      <c r="F13" s="76"/>
+      <c r="G13" s="77"/>
+      <c r="H13" s="2"/>
+      <c r="I13" s="57" t="s">
+        <v>19</v>
+      </c>
+      <c r="J13" s="58"/>
+      <c r="K13" s="58"/>
+      <c r="L13" s="58"/>
+      <c r="M13" s="59"/>
+      <c r="N13" s="60"/>
+    </row>
+    <row r="14" spans="2:14" ht="31.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B14" s="73" t="s">
+        <v>6</v>
+      </c>
+      <c r="C14" s="74"/>
+      <c r="D14" s="74" t="s">
+        <v>35</v>
+      </c>
+      <c r="E14" s="74"/>
+      <c r="F14" s="74" t="s">
         <v>7</v>
       </c>
-      <c r="C13" s="49"/>
-      <c r="D13" s="49"/>
-      <c r="E13" s="49"/>
-      <c r="F13" s="49"/>
-      <c r="G13" s="50"/>
-      <c r="H13" s="2"/>
-      <c r="I13" s="93" t="s">
-        <v>22</v>
-      </c>
-      <c r="J13" s="94"/>
-      <c r="K13" s="94"/>
-      <c r="L13" s="94"/>
-      <c r="M13" s="95"/>
-      <c r="N13" s="96"/>
-    </row>
-    <row r="14" spans="2:14" ht="31.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="46" t="s">
+      <c r="G14" s="78"/>
+      <c r="H14" s="3"/>
+      <c r="I14" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="J14" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="K14" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="L14" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="M14" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="N14" s="21" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="15" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B15" s="66" t="s">
         <v>8</v>
       </c>
-      <c r="C14" s="47"/>
-      <c r="D14" s="47" t="s">
+      <c r="C15" s="67"/>
+      <c r="D15" s="67">
+        <v>0</v>
+      </c>
+      <c r="E15" s="67"/>
+      <c r="F15" s="71">
+        <v>0</v>
+      </c>
+      <c r="G15" s="72"/>
+      <c r="H15" s="1"/>
+      <c r="I15" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="J15" s="24">
+        <v>0</v>
+      </c>
+      <c r="K15" s="24">
+        <v>0</v>
+      </c>
+      <c r="L15" s="24">
+        <v>0</v>
+      </c>
+      <c r="M15" s="24">
+        <v>0</v>
+      </c>
+      <c r="N15" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="2:14" ht="22.5" x14ac:dyDescent="0.25">
+      <c r="B16" s="66" t="s">
+        <v>9</v>
+      </c>
+      <c r="C16" s="67"/>
+      <c r="D16" s="67">
+        <v>0</v>
+      </c>
+      <c r="E16" s="67"/>
+      <c r="F16" s="71">
+        <v>0</v>
+      </c>
+      <c r="G16" s="72"/>
+      <c r="H16" s="1"/>
+      <c r="I16" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="J16" s="26">
+        <f>SUM(J17:J19)</f>
+        <v>0</v>
+      </c>
+      <c r="K16" s="26">
+        <f>SUM(K17:K19)</f>
+        <v>0</v>
+      </c>
+      <c r="L16" s="26">
+        <f>SUM(L17:L19)</f>
+        <v>0</v>
+      </c>
+      <c r="M16" s="26">
+        <f>SUM(M17:M19)</f>
+        <v>0</v>
+      </c>
+      <c r="N16" s="26">
+        <f>SUM(N17:N19)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="2:14" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="104" t="s">
+        <v>34</v>
+      </c>
+      <c r="C17" s="103"/>
+      <c r="D17" s="103" t="s">
+        <v>36</v>
+      </c>
+      <c r="E17" s="103"/>
+      <c r="F17" s="105">
+        <v>0</v>
+      </c>
+      <c r="G17" s="106"/>
+      <c r="H17" s="1"/>
+      <c r="I17" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="J17" s="27">
+        <v>0</v>
+      </c>
+      <c r="K17" s="27">
+        <v>0</v>
+      </c>
+      <c r="L17" s="27">
+        <v>0</v>
+      </c>
+      <c r="M17" s="27">
+        <v>0</v>
+      </c>
+      <c r="N17" s="28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="2:14" ht="23.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B18" s="107" t="s">
+        <v>37</v>
+      </c>
+      <c r="C18" s="108"/>
+      <c r="D18" s="108" t="s">
+        <v>17</v>
+      </c>
+      <c r="E18" s="108"/>
+      <c r="F18" s="109">
+        <v>0</v>
+      </c>
+      <c r="G18" s="110"/>
+      <c r="H18" s="1"/>
+      <c r="I18" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="J18" s="27">
+        <v>0</v>
+      </c>
+      <c r="K18" s="27">
+        <v>0</v>
+      </c>
+      <c r="L18" s="27">
+        <v>0</v>
+      </c>
+      <c r="M18" s="27">
+        <v>0</v>
+      </c>
+      <c r="N18" s="28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="2:14" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B19" s="63" t="s">
+        <v>10</v>
+      </c>
+      <c r="C19" s="64"/>
+      <c r="D19" s="64"/>
+      <c r="E19" s="65"/>
+      <c r="F19" s="61">
+        <f>SUM(F15:G18)</f>
+        <v>0</v>
+      </c>
+      <c r="G19" s="62"/>
+      <c r="H19" s="1"/>
+      <c r="I19" s="23" t="s">
         <v>38</v>
       </c>
-      <c r="E14" s="47"/>
-      <c r="F14" s="47" t="s">
-        <v>9</v>
-      </c>
-      <c r="G14" s="51"/>
-      <c r="H14" s="3"/>
-      <c r="I14" s="98" t="s">
-        <v>0</v>
-      </c>
-      <c r="J14" s="99" t="s">
-        <v>42</v>
-      </c>
-      <c r="K14" s="99" t="s">
-        <v>14</v>
-      </c>
-      <c r="L14" s="99" t="s">
-        <v>15</v>
-      </c>
-      <c r="M14" s="99" t="s">
-        <v>16</v>
-      </c>
-      <c r="N14" s="100" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="15" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="78" t="s">
-        <v>10</v>
-      </c>
-      <c r="C15" s="43"/>
-      <c r="D15" s="43">
-        <v>3</v>
-      </c>
-      <c r="E15" s="43"/>
-      <c r="F15" s="44">
-        <v>700000</v>
-      </c>
-      <c r="G15" s="45"/>
-      <c r="H15" s="1"/>
-      <c r="I15" s="97" t="s">
-        <v>13</v>
-      </c>
-      <c r="J15" s="91">
-        <v>8807988</v>
-      </c>
-      <c r="K15" s="91">
-        <v>9070728</v>
-      </c>
-      <c r="L15" s="91">
-        <v>9892902</v>
-      </c>
-      <c r="M15" s="91">
-        <v>9620090</v>
-      </c>
-      <c r="N15" s="92">
-        <v>9620090</v>
-      </c>
-    </row>
-    <row r="16" spans="2:14" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="B16" s="78" t="s">
-        <v>11</v>
-      </c>
-      <c r="C16" s="43"/>
-      <c r="D16" s="43">
-        <v>4</v>
-      </c>
-      <c r="E16" s="43"/>
-      <c r="F16" s="44">
-        <v>300000</v>
-      </c>
-      <c r="G16" s="45"/>
-      <c r="H16" s="1"/>
-      <c r="I16" s="88" t="s">
-        <v>45</v>
-      </c>
-      <c r="J16" s="89">
-        <f>SUM(J17:J19)</f>
-        <v>6300000</v>
-      </c>
-      <c r="K16" s="89">
-        <f t="shared" ref="K16:N16" si="0">SUM(K17:K19)</f>
-        <v>300000</v>
-      </c>
-      <c r="L16" s="89">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="M16" s="89">
-        <f t="shared" ref="M16" si="1">SUM(M17:M19)</f>
-        <v>0</v>
-      </c>
-      <c r="N16" s="90">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="2:14" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="19" t="s">
-        <v>37</v>
-      </c>
-      <c r="C17" s="18"/>
-      <c r="D17" s="18" t="s">
-        <v>39</v>
-      </c>
-      <c r="E17" s="18"/>
-      <c r="F17" s="20">
-        <v>5450000</v>
-      </c>
-      <c r="G17" s="21"/>
-      <c r="H17" s="1"/>
-      <c r="I17" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="J17" s="4">
-        <v>700000</v>
-      </c>
-      <c r="K17" s="4">
-        <v>300000</v>
-      </c>
-      <c r="L17" s="4">
-        <v>0</v>
-      </c>
-      <c r="M17" s="4">
-        <v>0</v>
-      </c>
-      <c r="N17" s="87">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="2:14" ht="23.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="22" t="s">
-        <v>40</v>
-      </c>
-      <c r="C18" s="23"/>
-      <c r="D18" s="23" t="s">
-        <v>20</v>
-      </c>
-      <c r="E18" s="23"/>
-      <c r="F18" s="24">
-        <v>150000</v>
-      </c>
-      <c r="G18" s="25"/>
-      <c r="H18" s="1"/>
-      <c r="I18" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="J18" s="4">
-        <v>5450000</v>
-      </c>
-      <c r="K18" s="4">
-        <v>0</v>
-      </c>
-      <c r="L18" s="4">
-        <v>0</v>
-      </c>
-      <c r="M18" s="4">
-        <v>0</v>
-      </c>
-      <c r="N18" s="87">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="2:14" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="75" t="s">
-        <v>12</v>
-      </c>
-      <c r="C19" s="76"/>
-      <c r="D19" s="76"/>
-      <c r="E19" s="77"/>
-      <c r="F19" s="73">
-        <f>SUM(F15:G18)</f>
-        <v>6600000</v>
-      </c>
-      <c r="G19" s="74"/>
-      <c r="H19" s="1"/>
-      <c r="I19" s="102" t="s">
-        <v>41</v>
-      </c>
-      <c r="J19" s="103">
-        <v>150000</v>
-      </c>
-      <c r="K19" s="103">
-        <v>0</v>
-      </c>
-      <c r="L19" s="103">
-        <v>0</v>
-      </c>
-      <c r="M19" s="103">
-        <v>0</v>
-      </c>
-      <c r="N19" s="104">
+      <c r="J19" s="29">
+        <v>0</v>
+      </c>
+      <c r="K19" s="29">
+        <v>0</v>
+      </c>
+      <c r="L19" s="29">
+        <v>0</v>
+      </c>
+      <c r="M19" s="29">
+        <v>0</v>
+      </c>
+      <c r="N19" s="30">
         <v>0</v>
       </c>
     </row>
     <row r="20" spans="2:14" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="101"/>
-      <c r="C20" s="101"/>
-      <c r="D20" s="101"/>
-      <c r="E20" s="101"/>
+      <c r="B20" s="22"/>
+      <c r="C20" s="22"/>
+      <c r="D20" s="22"/>
+      <c r="E20" s="22"/>
       <c r="F20" s="1"/>
       <c r="G20" s="1"/>
       <c r="H20" s="1"/>
-      <c r="I20" s="105" t="s">
-        <v>48</v>
-      </c>
-      <c r="J20" s="106"/>
-      <c r="K20" s="106"/>
-      <c r="L20" s="106"/>
-      <c r="M20" s="106"/>
-      <c r="N20" s="107"/>
+      <c r="I20" s="68" t="s">
+        <v>44</v>
+      </c>
+      <c r="J20" s="69"/>
+      <c r="K20" s="69"/>
+      <c r="L20" s="69"/>
+      <c r="M20" s="69"/>
+      <c r="N20" s="70"/>
     </row>
     <row r="21" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="22" spans="2:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="52" t="s">
-        <v>23</v>
-      </c>
-      <c r="C22" s="53"/>
-      <c r="D22" s="53"/>
-      <c r="E22" s="53"/>
-      <c r="F22" s="53"/>
-      <c r="G22" s="53"/>
-      <c r="H22" s="53"/>
-      <c r="I22" s="53"/>
-      <c r="J22" s="53"/>
-      <c r="K22" s="53"/>
-      <c r="L22" s="53"/>
-      <c r="M22" s="84"/>
-      <c r="N22" s="54"/>
+      <c r="B22" s="31" t="s">
+        <v>20</v>
+      </c>
+      <c r="C22" s="32"/>
+      <c r="D22" s="32"/>
+      <c r="E22" s="32"/>
+      <c r="F22" s="32"/>
+      <c r="G22" s="32"/>
+      <c r="H22" s="32"/>
+      <c r="I22" s="32"/>
+      <c r="J22" s="32"/>
+      <c r="K22" s="32"/>
+      <c r="L22" s="32"/>
+      <c r="M22" s="33"/>
+      <c r="N22" s="34"/>
     </row>
     <row r="23" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="24" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B24" s="55" t="s">
-        <v>24</v>
-      </c>
-      <c r="C24" s="56"/>
-      <c r="D24" s="56"/>
-      <c r="E24" s="56"/>
-      <c r="F24" s="56"/>
-      <c r="G24" s="56"/>
-      <c r="H24" s="57"/>
-      <c r="J24" s="58" t="s">
-        <v>25</v>
-      </c>
-      <c r="K24" s="59"/>
-      <c r="L24" s="59"/>
-      <c r="M24" s="85"/>
-      <c r="N24" s="60"/>
+      <c r="B24" s="35" t="s">
+        <v>21</v>
+      </c>
+      <c r="C24" s="36"/>
+      <c r="D24" s="36"/>
+      <c r="E24" s="36"/>
+      <c r="F24" s="36"/>
+      <c r="G24" s="36"/>
+      <c r="H24" s="37"/>
+      <c r="J24" s="38" t="s">
+        <v>22</v>
+      </c>
+      <c r="K24" s="39"/>
+      <c r="L24" s="39"/>
+      <c r="M24" s="40"/>
+      <c r="N24" s="41"/>
     </row>
     <row r="25" spans="2:14" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="10"/>
-      <c r="C25" s="5"/>
-      <c r="D25" s="5"/>
-      <c r="E25" s="5"/>
-      <c r="F25" s="5"/>
-      <c r="G25" s="5"/>
-      <c r="H25" s="11"/>
-      <c r="J25" s="61" t="s">
-        <v>26</v>
-      </c>
-      <c r="K25" s="62"/>
-      <c r="L25" s="62"/>
-      <c r="M25" s="86"/>
-      <c r="N25" s="63"/>
+      <c r="B25" s="9"/>
+      <c r="C25" s="4"/>
+      <c r="D25" s="4"/>
+      <c r="E25" s="4"/>
+      <c r="F25" s="4"/>
+      <c r="G25" s="4"/>
+      <c r="H25" s="10"/>
+      <c r="J25" s="42" t="s">
+        <v>23</v>
+      </c>
+      <c r="K25" s="43"/>
+      <c r="L25" s="43"/>
+      <c r="M25" s="44"/>
+      <c r="N25" s="45"/>
     </row>
     <row r="26" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B26" s="12"/>
-      <c r="C26" s="6"/>
-      <c r="D26" s="6"/>
-      <c r="E26" s="6"/>
-      <c r="F26" s="6"/>
-      <c r="G26" s="6"/>
-      <c r="H26" s="13"/>
-      <c r="J26" s="10"/>
-      <c r="K26" s="5"/>
-      <c r="L26" s="5"/>
-      <c r="M26" s="5"/>
-      <c r="N26" s="11"/>
+      <c r="B26" s="11"/>
+      <c r="C26" s="5"/>
+      <c r="D26" s="5"/>
+      <c r="E26" s="5"/>
+      <c r="F26" s="5"/>
+      <c r="G26" s="5"/>
+      <c r="H26" s="12"/>
+      <c r="J26" s="9"/>
+      <c r="K26" s="4"/>
+      <c r="L26" s="4"/>
+      <c r="M26" s="4"/>
+      <c r="N26" s="10"/>
     </row>
     <row r="27" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B27" s="12"/>
-      <c r="C27" s="6"/>
-      <c r="D27" s="6"/>
-      <c r="E27" s="6"/>
-      <c r="F27" s="6"/>
-      <c r="G27" s="6"/>
-      <c r="H27" s="13"/>
-      <c r="J27" s="12"/>
-      <c r="K27" s="6"/>
-      <c r="L27" s="6"/>
-      <c r="M27" s="6"/>
-      <c r="N27" s="13"/>
+      <c r="B27" s="11"/>
+      <c r="C27" s="5"/>
+      <c r="D27" s="5"/>
+      <c r="E27" s="5"/>
+      <c r="F27" s="5"/>
+      <c r="G27" s="5"/>
+      <c r="H27" s="12"/>
+      <c r="J27" s="11"/>
+      <c r="K27" s="5"/>
+      <c r="L27" s="5"/>
+      <c r="M27" s="5"/>
+      <c r="N27" s="12"/>
     </row>
     <row r="28" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B28" s="12"/>
-      <c r="C28" s="6"/>
-      <c r="D28" s="6"/>
-      <c r="E28" s="6"/>
-      <c r="F28" s="6"/>
-      <c r="G28" s="6"/>
-      <c r="H28" s="13"/>
-      <c r="J28" s="12"/>
-      <c r="K28" s="6"/>
-      <c r="L28" s="6"/>
-      <c r="M28" s="6"/>
-      <c r="N28" s="13"/>
+      <c r="B28" s="11"/>
+      <c r="C28" s="5"/>
+      <c r="D28" s="5"/>
+      <c r="E28" s="5"/>
+      <c r="F28" s="5"/>
+      <c r="G28" s="5"/>
+      <c r="H28" s="12"/>
+      <c r="J28" s="11"/>
+      <c r="K28" s="5"/>
+      <c r="L28" s="5"/>
+      <c r="M28" s="5"/>
+      <c r="N28" s="12"/>
     </row>
     <row r="29" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B29" s="12"/>
-      <c r="C29" s="6"/>
-      <c r="D29" s="6"/>
-      <c r="E29" s="6"/>
-      <c r="F29" s="6"/>
-      <c r="G29" s="6"/>
-      <c r="H29" s="13"/>
-      <c r="J29" s="12"/>
-      <c r="K29" s="6"/>
-      <c r="L29" s="6"/>
-      <c r="M29" s="6"/>
-      <c r="N29" s="13"/>
+      <c r="B29" s="11"/>
+      <c r="C29" s="5"/>
+      <c r="D29" s="5"/>
+      <c r="E29" s="5"/>
+      <c r="F29" s="5"/>
+      <c r="G29" s="5"/>
+      <c r="H29" s="12"/>
+      <c r="J29" s="11"/>
+      <c r="K29" s="5"/>
+      <c r="L29" s="5"/>
+      <c r="M29" s="5"/>
+      <c r="N29" s="12"/>
     </row>
     <row r="30" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B30" s="12"/>
-      <c r="C30" s="6"/>
-      <c r="D30" s="6"/>
-      <c r="E30" s="6"/>
-      <c r="F30" s="6"/>
-      <c r="G30" s="6"/>
-      <c r="H30" s="13"/>
-      <c r="J30" s="12"/>
-      <c r="K30" s="6"/>
-      <c r="L30" s="6"/>
-      <c r="M30" s="6"/>
-      <c r="N30" s="13"/>
+      <c r="B30" s="11"/>
+      <c r="C30" s="5"/>
+      <c r="D30" s="5"/>
+      <c r="E30" s="5"/>
+      <c r="F30" s="5"/>
+      <c r="G30" s="5"/>
+      <c r="H30" s="12"/>
+      <c r="J30" s="11"/>
+      <c r="K30" s="5"/>
+      <c r="L30" s="5"/>
+      <c r="M30" s="5"/>
+      <c r="N30" s="12"/>
     </row>
     <row r="31" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B31" s="12"/>
-      <c r="C31" s="6"/>
-      <c r="D31" s="6"/>
-      <c r="E31" s="6"/>
-      <c r="F31" s="6"/>
-      <c r="G31" s="6"/>
-      <c r="H31" s="13"/>
-      <c r="J31" s="12"/>
-      <c r="K31" s="6"/>
-      <c r="L31" s="6"/>
-      <c r="M31" s="6"/>
-      <c r="N31" s="13"/>
+      <c r="B31" s="11"/>
+      <c r="C31" s="5"/>
+      <c r="D31" s="5"/>
+      <c r="E31" s="5"/>
+      <c r="F31" s="5"/>
+      <c r="G31" s="5"/>
+      <c r="H31" s="12"/>
+      <c r="J31" s="11"/>
+      <c r="K31" s="5"/>
+      <c r="L31" s="5"/>
+      <c r="M31" s="5"/>
+      <c r="N31" s="12"/>
     </row>
     <row r="32" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B32" s="12"/>
-      <c r="C32" s="6"/>
-      <c r="D32" s="6"/>
-      <c r="E32" s="6"/>
-      <c r="F32" s="6"/>
-      <c r="G32" s="6"/>
-      <c r="H32" s="13"/>
-      <c r="J32" s="12"/>
-      <c r="K32" s="6"/>
-      <c r="L32" s="6"/>
-      <c r="M32" s="6"/>
-      <c r="N32" s="13"/>
+      <c r="B32" s="11"/>
+      <c r="C32" s="5"/>
+      <c r="D32" s="5"/>
+      <c r="E32" s="5"/>
+      <c r="F32" s="5"/>
+      <c r="G32" s="5"/>
+      <c r="H32" s="12"/>
+      <c r="J32" s="11"/>
+      <c r="K32" s="5"/>
+      <c r="L32" s="5"/>
+      <c r="M32" s="5"/>
+      <c r="N32" s="12"/>
     </row>
     <row r="33" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B33" s="12"/>
-      <c r="C33" s="6"/>
-      <c r="D33" s="6"/>
-      <c r="E33" s="6"/>
-      <c r="F33" s="6"/>
-      <c r="G33" s="6"/>
-      <c r="H33" s="13"/>
-      <c r="J33" s="12"/>
-      <c r="K33" s="6"/>
-      <c r="L33" s="6"/>
-      <c r="M33" s="6"/>
-      <c r="N33" s="13"/>
+      <c r="B33" s="11"/>
+      <c r="C33" s="5"/>
+      <c r="D33" s="5"/>
+      <c r="E33" s="5"/>
+      <c r="F33" s="5"/>
+      <c r="G33" s="5"/>
+      <c r="H33" s="12"/>
+      <c r="J33" s="11"/>
+      <c r="K33" s="5"/>
+      <c r="L33" s="5"/>
+      <c r="M33" s="5"/>
+      <c r="N33" s="12"/>
     </row>
     <row r="34" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B34" s="12"/>
-      <c r="C34" s="6"/>
-      <c r="D34" s="6"/>
-      <c r="E34" s="6"/>
-      <c r="F34" s="6"/>
-      <c r="G34" s="6"/>
-      <c r="H34" s="13"/>
-      <c r="J34" s="12"/>
-      <c r="K34" s="6"/>
-      <c r="L34" s="6"/>
-      <c r="M34" s="6"/>
-      <c r="N34" s="13"/>
+      <c r="B34" s="11"/>
+      <c r="C34" s="5"/>
+      <c r="D34" s="5"/>
+      <c r="E34" s="5"/>
+      <c r="F34" s="5"/>
+      <c r="G34" s="5"/>
+      <c r="H34" s="12"/>
+      <c r="J34" s="11"/>
+      <c r="K34" s="5"/>
+      <c r="L34" s="5"/>
+      <c r="M34" s="5"/>
+      <c r="N34" s="12"/>
     </row>
     <row r="35" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B35" s="12"/>
-      <c r="C35" s="6"/>
-      <c r="D35" s="6"/>
-      <c r="E35" s="6"/>
-      <c r="F35" s="6"/>
-      <c r="G35" s="6"/>
-      <c r="H35" s="13"/>
-      <c r="J35" s="12"/>
-      <c r="K35" s="6"/>
-      <c r="L35" s="6"/>
-      <c r="M35" s="6"/>
-      <c r="N35" s="13"/>
+      <c r="B35" s="11"/>
+      <c r="C35" s="5"/>
+      <c r="D35" s="5"/>
+      <c r="E35" s="5"/>
+      <c r="F35" s="5"/>
+      <c r="G35" s="5"/>
+      <c r="H35" s="12"/>
+      <c r="J35" s="11"/>
+      <c r="K35" s="5"/>
+      <c r="L35" s="5"/>
+      <c r="M35" s="5"/>
+      <c r="N35" s="12"/>
     </row>
     <row r="36" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B36" s="12"/>
-      <c r="C36" s="6"/>
-      <c r="D36" s="6"/>
-      <c r="E36" s="6"/>
-      <c r="F36" s="6"/>
-      <c r="G36" s="6"/>
-      <c r="H36" s="13"/>
-      <c r="J36" s="12"/>
-      <c r="K36" s="6"/>
-      <c r="L36" s="6"/>
-      <c r="M36" s="6"/>
-      <c r="N36" s="13"/>
+      <c r="B36" s="11"/>
+      <c r="C36" s="5"/>
+      <c r="D36" s="5"/>
+      <c r="E36" s="5"/>
+      <c r="F36" s="5"/>
+      <c r="G36" s="5"/>
+      <c r="H36" s="12"/>
+      <c r="J36" s="11"/>
+      <c r="K36" s="5"/>
+      <c r="L36" s="5"/>
+      <c r="M36" s="5"/>
+      <c r="N36" s="12"/>
     </row>
     <row r="37" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B37" s="14"/>
-      <c r="C37" s="15"/>
-      <c r="D37" s="15"/>
-      <c r="E37" s="15"/>
-      <c r="F37" s="15"/>
-      <c r="G37" s="15"/>
-      <c r="H37" s="16"/>
-      <c r="J37" s="14"/>
-      <c r="K37" s="15"/>
-      <c r="L37" s="15"/>
-      <c r="M37" s="15"/>
-      <c r="N37" s="16"/>
+      <c r="B37" s="13"/>
+      <c r="C37" s="14"/>
+      <c r="D37" s="14"/>
+      <c r="E37" s="14"/>
+      <c r="F37" s="14"/>
+      <c r="G37" s="14"/>
+      <c r="H37" s="15"/>
+      <c r="J37" s="13"/>
+      <c r="K37" s="14"/>
+      <c r="L37" s="14"/>
+      <c r="M37" s="14"/>
+      <c r="N37" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="40">
+    <mergeCell ref="D17:E17"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="F17:G17"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="F18:G18"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="D4:N4"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B8:C9"/>
+    <mergeCell ref="D8:F8"/>
+    <mergeCell ref="G8:N8"/>
+    <mergeCell ref="D9:F9"/>
+    <mergeCell ref="G9:N9"/>
+    <mergeCell ref="I6:J6"/>
+    <mergeCell ref="K6:N6"/>
+    <mergeCell ref="D6:H6"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="F15:G15"/>
+    <mergeCell ref="F16:G16"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B13:G13"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="F14:G14"/>
     <mergeCell ref="B22:N22"/>
     <mergeCell ref="B24:H24"/>
     <mergeCell ref="J24:N24"/>
@@ -2539,33 +2557,9 @@
     <mergeCell ref="B16:C16"/>
     <mergeCell ref="D15:E15"/>
     <mergeCell ref="I20:N20"/>
-    <mergeCell ref="D16:E16"/>
-    <mergeCell ref="F15:G15"/>
-    <mergeCell ref="F16:G16"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="B13:G13"/>
-    <mergeCell ref="D14:E14"/>
-    <mergeCell ref="F14:G14"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="D4:N4"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="B8:C9"/>
-    <mergeCell ref="D8:F8"/>
-    <mergeCell ref="G8:N8"/>
-    <mergeCell ref="D9:F9"/>
-    <mergeCell ref="G9:N9"/>
-    <mergeCell ref="I6:J6"/>
-    <mergeCell ref="K6:N6"/>
-    <mergeCell ref="D6:H6"/>
-    <mergeCell ref="D17:E17"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="F17:G17"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="F18:G18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup scale="57" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
 </file>
@@ -2584,58 +2578,58 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" s="7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B3" s="7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="7" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
+      <c r="B4" s="7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="B2" s="8">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="8" t="s">
+      <c r="B5" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="B3" s="8">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="B4" s="8">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="B5" s="8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="B6" s="8">
+      <c r="B6" s="7">
         <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="17" t="s">
-        <v>46</v>
-      </c>
-      <c r="B7" s="17">
+      <c r="A7" s="16" t="s">
+        <v>43</v>
+      </c>
+      <c r="B7" s="16">
         <v>2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
changed template for tap legacy system dispositions report
git-svn-id: svn://107.170.10.188:8080/Semoss/trunk@2882 ef391c1c-ee15-45f7-b1d6-dde3d27a2169

Former-commit-id: 28714f29f84f44a92cdf72f2c478b43af34d395e
</commit_message>
<xml_diff>
--- a/export/Reports/TAP_Legacy_System_Dispositions_Template.xlsx
+++ b/export/Reports/TAP_Legacy_System_Dispositions_Template.xlsx
@@ -990,6 +990,129 @@
     <xf numFmtId="44" fontId="8" fillId="0" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="7" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="7" fillId="0" borderId="18" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="7" fillId="0" borderId="19" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="7" fillId="0" borderId="20" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="7" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="7" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1098,9 +1221,6 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="15" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1109,126 +1229,6 @@
     </xf>
     <xf numFmtId="0" fontId="15" fillId="5" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="7" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="7" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="5" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="7" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="7" fillId="0" borderId="18" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="7" fillId="0" borderId="19" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="7" fillId="0" borderId="20" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1447,11 +1447,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="535397864"/>
-        <c:axId val="535398256"/>
+        <c:axId val="539701144"/>
+        <c:axId val="539705064"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="535397864"/>
+        <c:axId val="539701144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1460,7 +1460,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="535398256"/>
+        <c:crossAx val="539705064"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1468,7 +1468,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="535398256"/>
+        <c:axId val="539705064"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1479,7 +1479,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="535397864"/>
+        <c:crossAx val="539701144"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1522,61 +1522,6 @@
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>63299</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>66675</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>495300</xdr:colOff>
-      <xdr:row>36</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Picture 2"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="225224" y="6181725"/>
-          <a:ext cx="4089601" cy="2438400"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>9</xdr:col>
@@ -1601,7 +1546,7 @@
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1899,7 +1844,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:N37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A20" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="I28" sqref="I28"/>
     </sheetView>
   </sheetViews>
@@ -1916,178 +1861,178 @@
   <sheetData>
     <row r="1" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:14" ht="72" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="46" t="s">
+      <c r="B2" s="87" t="s">
         <v>31</v>
       </c>
-      <c r="C2" s="47"/>
-      <c r="D2" s="48" t="s">
+      <c r="C2" s="88"/>
+      <c r="D2" s="89" t="s">
         <v>32</v>
       </c>
-      <c r="E2" s="49"/>
-      <c r="F2" s="49"/>
-      <c r="G2" s="49"/>
-      <c r="H2" s="49"/>
-      <c r="I2" s="49"/>
-      <c r="J2" s="49"/>
-      <c r="K2" s="49"/>
-      <c r="L2" s="49"/>
-      <c r="M2" s="50"/>
-      <c r="N2" s="51"/>
+      <c r="E2" s="90"/>
+      <c r="F2" s="90"/>
+      <c r="G2" s="90"/>
+      <c r="H2" s="90"/>
+      <c r="I2" s="90"/>
+      <c r="J2" s="90"/>
+      <c r="K2" s="90"/>
+      <c r="L2" s="90"/>
+      <c r="M2" s="91"/>
+      <c r="N2" s="92"/>
     </row>
     <row r="3" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="2:14" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="79" t="s">
+      <c r="B4" s="39" t="s">
         <v>46</v>
       </c>
-      <c r="C4" s="80"/>
-      <c r="D4" s="81" t="s">
+      <c r="C4" s="40"/>
+      <c r="D4" s="41" t="s">
         <v>1</v>
       </c>
-      <c r="E4" s="81"/>
-      <c r="F4" s="81"/>
-      <c r="G4" s="81"/>
-      <c r="H4" s="81"/>
-      <c r="I4" s="81"/>
-      <c r="J4" s="81"/>
-      <c r="K4" s="81"/>
-      <c r="L4" s="81"/>
-      <c r="M4" s="82"/>
-      <c r="N4" s="83"/>
+      <c r="E4" s="41"/>
+      <c r="F4" s="41"/>
+      <c r="G4" s="41"/>
+      <c r="H4" s="41"/>
+      <c r="I4" s="41"/>
+      <c r="J4" s="41"/>
+      <c r="K4" s="41"/>
+      <c r="L4" s="41"/>
+      <c r="M4" s="42"/>
+      <c r="N4" s="43"/>
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B5" s="52" t="s">
+      <c r="B5" s="93" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="53"/>
-      <c r="D5" s="54" t="s">
+      <c r="C5" s="94"/>
+      <c r="D5" s="95" t="s">
         <v>47</v>
       </c>
-      <c r="E5" s="54"/>
-      <c r="F5" s="54"/>
-      <c r="G5" s="54"/>
-      <c r="H5" s="54"/>
-      <c r="I5" s="54"/>
-      <c r="J5" s="54"/>
-      <c r="K5" s="54"/>
-      <c r="L5" s="54"/>
-      <c r="M5" s="55"/>
-      <c r="N5" s="56"/>
+      <c r="E5" s="95"/>
+      <c r="F5" s="95"/>
+      <c r="G5" s="95"/>
+      <c r="H5" s="95"/>
+      <c r="I5" s="95"/>
+      <c r="J5" s="95"/>
+      <c r="K5" s="95"/>
+      <c r="L5" s="95"/>
+      <c r="M5" s="96"/>
+      <c r="N5" s="97"/>
     </row>
     <row r="6" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="84" t="s">
+      <c r="B6" s="44" t="s">
         <v>16</v>
       </c>
-      <c r="C6" s="85"/>
-      <c r="D6" s="102">
+      <c r="C6" s="45"/>
+      <c r="D6" s="62">
         <v>42005</v>
       </c>
-      <c r="E6" s="102"/>
-      <c r="F6" s="102"/>
-      <c r="G6" s="102"/>
-      <c r="H6" s="102"/>
-      <c r="I6" s="97" t="s">
+      <c r="E6" s="62"/>
+      <c r="F6" s="62"/>
+      <c r="G6" s="62"/>
+      <c r="H6" s="62"/>
+      <c r="I6" s="57" t="s">
         <v>40</v>
       </c>
-      <c r="J6" s="97"/>
-      <c r="K6" s="98">
+      <c r="J6" s="57"/>
+      <c r="K6" s="58">
         <v>42005</v>
       </c>
-      <c r="L6" s="99"/>
-      <c r="M6" s="100"/>
-      <c r="N6" s="101"/>
+      <c r="L6" s="59"/>
+      <c r="M6" s="60"/>
+      <c r="N6" s="61"/>
     </row>
     <row r="7" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="8" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B8" s="86" t="s">
+      <c r="B8" s="46" t="s">
         <v>3</v>
       </c>
-      <c r="C8" s="87"/>
-      <c r="D8" s="90" t="s">
+      <c r="C8" s="47"/>
+      <c r="D8" s="50" t="s">
         <v>2</v>
       </c>
-      <c r="E8" s="90"/>
-      <c r="F8" s="90"/>
-      <c r="G8" s="90" t="s">
+      <c r="E8" s="50"/>
+      <c r="F8" s="50"/>
+      <c r="G8" s="50" t="s">
         <v>4</v>
       </c>
-      <c r="H8" s="90"/>
-      <c r="I8" s="90"/>
-      <c r="J8" s="90"/>
-      <c r="K8" s="90"/>
-      <c r="L8" s="90"/>
-      <c r="M8" s="91"/>
-      <c r="N8" s="92"/>
+      <c r="H8" s="50"/>
+      <c r="I8" s="50"/>
+      <c r="J8" s="50"/>
+      <c r="K8" s="50"/>
+      <c r="L8" s="50"/>
+      <c r="M8" s="51"/>
+      <c r="N8" s="52"/>
     </row>
     <row r="9" spans="2:14" ht="40.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="88"/>
-      <c r="C9" s="89"/>
-      <c r="D9" s="93" t="s">
+      <c r="B9" s="48"/>
+      <c r="C9" s="49"/>
+      <c r="D9" s="53" t="s">
         <v>48</v>
       </c>
-      <c r="E9" s="93"/>
-      <c r="F9" s="93"/>
-      <c r="G9" s="94" t="s">
+      <c r="E9" s="53"/>
+      <c r="F9" s="53"/>
+      <c r="G9" s="54" t="s">
         <v>49</v>
       </c>
-      <c r="H9" s="94"/>
-      <c r="I9" s="94"/>
-      <c r="J9" s="94"/>
-      <c r="K9" s="94"/>
-      <c r="L9" s="94"/>
-      <c r="M9" s="95"/>
-      <c r="N9" s="96"/>
+      <c r="H9" s="54"/>
+      <c r="I9" s="54"/>
+      <c r="J9" s="54"/>
+      <c r="K9" s="54"/>
+      <c r="L9" s="54"/>
+      <c r="M9" s="55"/>
+      <c r="N9" s="56"/>
     </row>
     <row r="10" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="11" spans="2:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="31" t="s">
+      <c r="B11" s="72" t="s">
         <v>18</v>
       </c>
-      <c r="C11" s="32"/>
-      <c r="D11" s="32"/>
-      <c r="E11" s="32"/>
-      <c r="F11" s="32"/>
-      <c r="G11" s="32"/>
-      <c r="H11" s="32"/>
-      <c r="I11" s="32"/>
-      <c r="J11" s="32"/>
-      <c r="K11" s="32"/>
-      <c r="L11" s="32"/>
-      <c r="M11" s="33"/>
-      <c r="N11" s="34"/>
+      <c r="C11" s="73"/>
+      <c r="D11" s="73"/>
+      <c r="E11" s="73"/>
+      <c r="F11" s="73"/>
+      <c r="G11" s="73"/>
+      <c r="H11" s="73"/>
+      <c r="I11" s="73"/>
+      <c r="J11" s="73"/>
+      <c r="K11" s="73"/>
+      <c r="L11" s="73"/>
+      <c r="M11" s="74"/>
+      <c r="N11" s="75"/>
     </row>
     <row r="12" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="13" spans="2:14" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="75" t="s">
+      <c r="B13" s="68" t="s">
         <v>5</v>
       </c>
-      <c r="C13" s="76"/>
-      <c r="D13" s="76"/>
-      <c r="E13" s="76"/>
-      <c r="F13" s="76"/>
-      <c r="G13" s="77"/>
+      <c r="C13" s="69"/>
+      <c r="D13" s="69"/>
+      <c r="E13" s="69"/>
+      <c r="F13" s="69"/>
+      <c r="G13" s="70"/>
       <c r="H13" s="2"/>
-      <c r="I13" s="57" t="s">
+      <c r="I13" s="98" t="s">
         <v>19</v>
       </c>
-      <c r="J13" s="58"/>
-      <c r="K13" s="58"/>
-      <c r="L13" s="58"/>
-      <c r="M13" s="59"/>
-      <c r="N13" s="60"/>
+      <c r="J13" s="99"/>
+      <c r="K13" s="99"/>
+      <c r="L13" s="99"/>
+      <c r="M13" s="100"/>
+      <c r="N13" s="101"/>
     </row>
     <row r="14" spans="2:14" ht="31.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="73" t="s">
+      <c r="B14" s="66" t="s">
         <v>6</v>
       </c>
-      <c r="C14" s="74"/>
-      <c r="D14" s="74" t="s">
+      <c r="C14" s="67"/>
+      <c r="D14" s="67" t="s">
         <v>35</v>
       </c>
-      <c r="E14" s="74"/>
-      <c r="F14" s="74" t="s">
+      <c r="E14" s="67"/>
+      <c r="F14" s="67" t="s">
         <v>7</v>
       </c>
-      <c r="G14" s="78"/>
+      <c r="G14" s="71"/>
       <c r="H14" s="3"/>
       <c r="I14" s="19" t="s">
         <v>0</v>
@@ -2109,18 +2054,18 @@
       </c>
     </row>
     <row r="15" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="66" t="s">
+      <c r="B15" s="107" t="s">
         <v>8</v>
       </c>
-      <c r="C15" s="67"/>
-      <c r="D15" s="67">
-        <v>0</v>
-      </c>
-      <c r="E15" s="67"/>
-      <c r="F15" s="71">
-        <v>0</v>
-      </c>
-      <c r="G15" s="72"/>
+      <c r="C15" s="63"/>
+      <c r="D15" s="63">
+        <v>0</v>
+      </c>
+      <c r="E15" s="63"/>
+      <c r="F15" s="64">
+        <v>0</v>
+      </c>
+      <c r="G15" s="65"/>
       <c r="H15" s="1"/>
       <c r="I15" s="18" t="s">
         <v>11</v>
@@ -2142,18 +2087,18 @@
       </c>
     </row>
     <row r="16" spans="2:14" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="B16" s="66" t="s">
+      <c r="B16" s="107" t="s">
         <v>9</v>
       </c>
-      <c r="C16" s="67"/>
-      <c r="D16" s="67">
-        <v>0</v>
-      </c>
-      <c r="E16" s="67"/>
-      <c r="F16" s="71">
-        <v>0</v>
-      </c>
-      <c r="G16" s="72"/>
+      <c r="C16" s="63"/>
+      <c r="D16" s="63">
+        <v>0</v>
+      </c>
+      <c r="E16" s="63"/>
+      <c r="F16" s="64">
+        <v>0</v>
+      </c>
+      <c r="G16" s="65"/>
       <c r="H16" s="1"/>
       <c r="I16" s="17" t="s">
         <v>42</v>
@@ -2180,18 +2125,18 @@
       </c>
     </row>
     <row r="17" spans="2:14" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="104" t="s">
+      <c r="B17" s="32" t="s">
         <v>34</v>
       </c>
-      <c r="C17" s="103"/>
-      <c r="D17" s="103" t="s">
+      <c r="C17" s="31"/>
+      <c r="D17" s="31" t="s">
         <v>36</v>
       </c>
-      <c r="E17" s="103"/>
-      <c r="F17" s="105">
-        <v>0</v>
-      </c>
-      <c r="G17" s="106"/>
+      <c r="E17" s="31"/>
+      <c r="F17" s="33">
+        <v>0</v>
+      </c>
+      <c r="G17" s="34"/>
       <c r="H17" s="1"/>
       <c r="I17" s="8" t="s">
         <v>33</v>
@@ -2213,18 +2158,18 @@
       </c>
     </row>
     <row r="18" spans="2:14" ht="23.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="107" t="s">
+      <c r="B18" s="35" t="s">
         <v>37</v>
       </c>
-      <c r="C18" s="108"/>
-      <c r="D18" s="108" t="s">
+      <c r="C18" s="36"/>
+      <c r="D18" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="E18" s="108"/>
-      <c r="F18" s="109">
-        <v>0</v>
-      </c>
-      <c r="G18" s="110"/>
+      <c r="E18" s="36"/>
+      <c r="F18" s="37">
+        <v>0</v>
+      </c>
+      <c r="G18" s="38"/>
       <c r="H18" s="1"/>
       <c r="I18" s="8" t="s">
         <v>45</v>
@@ -2246,17 +2191,17 @@
       </c>
     </row>
     <row r="19" spans="2:14" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="63" t="s">
+      <c r="B19" s="104" t="s">
         <v>10</v>
       </c>
-      <c r="C19" s="64"/>
-      <c r="D19" s="64"/>
-      <c r="E19" s="65"/>
-      <c r="F19" s="61">
+      <c r="C19" s="105"/>
+      <c r="D19" s="105"/>
+      <c r="E19" s="106"/>
+      <c r="F19" s="102">
         <f>SUM(F15:G18)</f>
         <v>0</v>
       </c>
-      <c r="G19" s="62"/>
+      <c r="G19" s="103"/>
       <c r="H19" s="1"/>
       <c r="I19" s="23" t="s">
         <v>38</v>
@@ -2285,51 +2230,51 @@
       <c r="F20" s="1"/>
       <c r="G20" s="1"/>
       <c r="H20" s="1"/>
-      <c r="I20" s="68" t="s">
+      <c r="I20" s="108" t="s">
         <v>44</v>
       </c>
-      <c r="J20" s="69"/>
-      <c r="K20" s="69"/>
-      <c r="L20" s="69"/>
-      <c r="M20" s="69"/>
-      <c r="N20" s="70"/>
+      <c r="J20" s="109"/>
+      <c r="K20" s="109"/>
+      <c r="L20" s="109"/>
+      <c r="M20" s="109"/>
+      <c r="N20" s="110"/>
     </row>
     <row r="21" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="22" spans="2:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="31" t="s">
+      <c r="B22" s="72" t="s">
         <v>20</v>
       </c>
-      <c r="C22" s="32"/>
-      <c r="D22" s="32"/>
-      <c r="E22" s="32"/>
-      <c r="F22" s="32"/>
-      <c r="G22" s="32"/>
-      <c r="H22" s="32"/>
-      <c r="I22" s="32"/>
-      <c r="J22" s="32"/>
-      <c r="K22" s="32"/>
-      <c r="L22" s="32"/>
-      <c r="M22" s="33"/>
-      <c r="N22" s="34"/>
+      <c r="C22" s="73"/>
+      <c r="D22" s="73"/>
+      <c r="E22" s="73"/>
+      <c r="F22" s="73"/>
+      <c r="G22" s="73"/>
+      <c r="H22" s="73"/>
+      <c r="I22" s="73"/>
+      <c r="J22" s="73"/>
+      <c r="K22" s="73"/>
+      <c r="L22" s="73"/>
+      <c r="M22" s="74"/>
+      <c r="N22" s="75"/>
     </row>
     <row r="23" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="24" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B24" s="35" t="s">
+      <c r="B24" s="76" t="s">
         <v>21</v>
       </c>
-      <c r="C24" s="36"/>
-      <c r="D24" s="36"/>
-      <c r="E24" s="36"/>
-      <c r="F24" s="36"/>
-      <c r="G24" s="36"/>
-      <c r="H24" s="37"/>
-      <c r="J24" s="38" t="s">
+      <c r="C24" s="77"/>
+      <c r="D24" s="77"/>
+      <c r="E24" s="77"/>
+      <c r="F24" s="77"/>
+      <c r="G24" s="77"/>
+      <c r="H24" s="78"/>
+      <c r="J24" s="79" t="s">
         <v>22</v>
       </c>
-      <c r="K24" s="39"/>
-      <c r="L24" s="39"/>
-      <c r="M24" s="40"/>
-      <c r="N24" s="41"/>
+      <c r="K24" s="80"/>
+      <c r="L24" s="80"/>
+      <c r="M24" s="81"/>
+      <c r="N24" s="82"/>
     </row>
     <row r="25" spans="2:14" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B25" s="9"/>
@@ -2339,13 +2284,13 @@
       <c r="F25" s="4"/>
       <c r="G25" s="4"/>
       <c r="H25" s="10"/>
-      <c r="J25" s="42" t="s">
+      <c r="J25" s="83" t="s">
         <v>23</v>
       </c>
-      <c r="K25" s="43"/>
-      <c r="L25" s="43"/>
-      <c r="M25" s="44"/>
-      <c r="N25" s="45"/>
+      <c r="K25" s="84"/>
+      <c r="L25" s="84"/>
+      <c r="M25" s="85"/>
+      <c r="N25" s="86"/>
     </row>
     <row r="26" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B26" s="11"/>
@@ -2517,30 +2462,6 @@
     </row>
   </sheetData>
   <mergeCells count="40">
-    <mergeCell ref="D17:E17"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="F17:G17"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="F18:G18"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="D4:N4"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="B8:C9"/>
-    <mergeCell ref="D8:F8"/>
-    <mergeCell ref="G8:N8"/>
-    <mergeCell ref="D9:F9"/>
-    <mergeCell ref="G9:N9"/>
-    <mergeCell ref="I6:J6"/>
-    <mergeCell ref="K6:N6"/>
-    <mergeCell ref="D6:H6"/>
-    <mergeCell ref="D16:E16"/>
-    <mergeCell ref="F15:G15"/>
-    <mergeCell ref="F16:G16"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="B13:G13"/>
-    <mergeCell ref="D14:E14"/>
-    <mergeCell ref="F14:G14"/>
     <mergeCell ref="B22:N22"/>
     <mergeCell ref="B24:H24"/>
     <mergeCell ref="J24:N24"/>
@@ -2557,6 +2478,30 @@
     <mergeCell ref="B16:C16"/>
     <mergeCell ref="D15:E15"/>
     <mergeCell ref="I20:N20"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="F15:G15"/>
+    <mergeCell ref="F16:G16"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B13:G13"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="F14:G14"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="D4:N4"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B8:C9"/>
+    <mergeCell ref="D8:F8"/>
+    <mergeCell ref="G8:N8"/>
+    <mergeCell ref="D9:F9"/>
+    <mergeCell ref="G9:N9"/>
+    <mergeCell ref="I6:J6"/>
+    <mergeCell ref="K6:N6"/>
+    <mergeCell ref="D6:H6"/>
+    <mergeCell ref="D17:E17"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="F17:G17"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="F18:G18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="57" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
updated formatting for template
git-svn-id: svn://107.170.10.188:8080/Semoss/trunk@2898 ef391c1c-ee15-45f7-b1d6-dde3d27a2169

Former-commit-id: abd7ec496bdba8ac51ce1c8902517892ab55f693
</commit_message>
<xml_diff>
--- a/export/Reports/TAP_Legacy_System_Dispositions_Template.xlsx
+++ b/export/Reports/TAP_Legacy_System_Dispositions_Template.xlsx
@@ -1087,273 +1087,273 @@
     <xf numFmtId="44" fontId="8" fillId="0" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="5" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="44" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="7" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="7" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="7" fillId="0" borderId="33" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="7" fillId="0" borderId="34" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyBorder="1"/>
+    <xf numFmtId="44" fontId="7" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="7" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="7" fillId="0" borderId="33" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="7" fillId="0" borderId="34" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="44" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -1571,11 +1571,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="492023216"/>
-        <c:axId val="492023608"/>
+        <c:axId val="554629216"/>
+        <c:axId val="554629608"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="492023216"/>
+        <c:axId val="554629216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1584,7 +1584,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="492023608"/>
+        <c:crossAx val="554629608"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1592,7 +1592,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="492023608"/>
+        <c:axId val="554629608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1603,7 +1603,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="492023216"/>
+        <c:crossAx val="554629216"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1649,15 +1649,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>10585</xdr:colOff>
+      <xdr:colOff>23284</xdr:colOff>
       <xdr:row>26</xdr:row>
-      <xdr:rowOff>19051</xdr:rowOff>
+      <xdr:rowOff>50801</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>963085</xdr:colOff>
+      <xdr:colOff>977899</xdr:colOff>
       <xdr:row>37</xdr:row>
-      <xdr:rowOff>148167</xdr:rowOff>
+      <xdr:rowOff>139700</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1969,8 +1969,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="B1:O38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="E29" sqref="E29"/>
+    <sheetView tabSelected="1" topLeftCell="F21" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="J27" sqref="J27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1988,187 +1988,187 @@
   <sheetData>
     <row r="1" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:15" ht="72" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="80" t="s">
+      <c r="B2" s="42" t="s">
         <v>31</v>
       </c>
-      <c r="C2" s="81"/>
-      <c r="D2" s="82"/>
-      <c r="E2" s="50" t="s">
+      <c r="C2" s="43"/>
+      <c r="D2" s="44"/>
+      <c r="E2" s="60" t="s">
         <v>32</v>
       </c>
-      <c r="F2" s="51"/>
-      <c r="G2" s="51"/>
-      <c r="H2" s="51"/>
-      <c r="I2" s="51"/>
-      <c r="J2" s="51"/>
-      <c r="K2" s="51"/>
-      <c r="L2" s="51"/>
-      <c r="M2" s="51"/>
-      <c r="N2" s="52"/>
-      <c r="O2" s="53"/>
+      <c r="F2" s="61"/>
+      <c r="G2" s="61"/>
+      <c r="H2" s="61"/>
+      <c r="I2" s="61"/>
+      <c r="J2" s="61"/>
+      <c r="K2" s="61"/>
+      <c r="L2" s="61"/>
+      <c r="M2" s="61"/>
+      <c r="N2" s="62"/>
+      <c r="O2" s="63"/>
     </row>
     <row r="3" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="2:15" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="83" t="s">
+      <c r="B4" s="45" t="s">
         <v>46</v>
       </c>
-      <c r="C4" s="84"/>
-      <c r="D4" s="85"/>
-      <c r="E4" s="70" t="s">
+      <c r="C4" s="46"/>
+      <c r="D4" s="47"/>
+      <c r="E4" s="77" t="s">
         <v>1</v>
       </c>
-      <c r="F4" s="71"/>
-      <c r="G4" s="71"/>
-      <c r="H4" s="71"/>
-      <c r="I4" s="71"/>
-      <c r="J4" s="71"/>
-      <c r="K4" s="71"/>
-      <c r="L4" s="71"/>
-      <c r="M4" s="71"/>
-      <c r="N4" s="72"/>
-      <c r="O4" s="73"/>
+      <c r="F4" s="78"/>
+      <c r="G4" s="78"/>
+      <c r="H4" s="78"/>
+      <c r="I4" s="78"/>
+      <c r="J4" s="78"/>
+      <c r="K4" s="78"/>
+      <c r="L4" s="78"/>
+      <c r="M4" s="78"/>
+      <c r="N4" s="79"/>
+      <c r="O4" s="80"/>
     </row>
     <row r="5" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="86" t="s">
+      <c r="B5" s="48" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="87"/>
-      <c r="D5" s="88"/>
-      <c r="E5" s="54" t="s">
+      <c r="C5" s="49"/>
+      <c r="D5" s="50"/>
+      <c r="E5" s="64" t="s">
         <v>47</v>
       </c>
-      <c r="F5" s="55"/>
-      <c r="G5" s="55"/>
-      <c r="H5" s="55"/>
-      <c r="I5" s="55"/>
-      <c r="J5" s="55"/>
-      <c r="K5" s="55"/>
-      <c r="L5" s="55"/>
-      <c r="M5" s="55"/>
-      <c r="N5" s="56"/>
-      <c r="O5" s="57"/>
+      <c r="F5" s="65"/>
+      <c r="G5" s="65"/>
+      <c r="H5" s="65"/>
+      <c r="I5" s="65"/>
+      <c r="J5" s="65"/>
+      <c r="K5" s="65"/>
+      <c r="L5" s="65"/>
+      <c r="M5" s="65"/>
+      <c r="N5" s="66"/>
+      <c r="O5" s="67"/>
     </row>
     <row r="6" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="89" t="s">
+      <c r="B6" s="51" t="s">
         <v>16</v>
       </c>
-      <c r="C6" s="90"/>
-      <c r="D6" s="91"/>
-      <c r="E6" s="45">
+      <c r="C6" s="52"/>
+      <c r="D6" s="53"/>
+      <c r="E6" s="107">
         <v>42005</v>
       </c>
-      <c r="F6" s="46"/>
-      <c r="G6" s="46"/>
-      <c r="H6" s="46"/>
-      <c r="I6" s="46"/>
-      <c r="J6" s="40" t="s">
+      <c r="F6" s="108"/>
+      <c r="G6" s="108"/>
+      <c r="H6" s="108"/>
+      <c r="I6" s="108"/>
+      <c r="J6" s="102" t="s">
         <v>40</v>
       </c>
-      <c r="K6" s="40"/>
-      <c r="L6" s="41">
+      <c r="K6" s="102"/>
+      <c r="L6" s="103">
         <v>42005</v>
       </c>
-      <c r="M6" s="42"/>
-      <c r="N6" s="43"/>
-      <c r="O6" s="44"/>
+      <c r="M6" s="104"/>
+      <c r="N6" s="105"/>
+      <c r="O6" s="106"/>
     </row>
     <row r="7" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="8" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="92" t="s">
+      <c r="B8" s="54" t="s">
         <v>3</v>
       </c>
-      <c r="C8" s="93"/>
-      <c r="D8" s="94"/>
-      <c r="E8" s="74" t="s">
+      <c r="C8" s="55"/>
+      <c r="D8" s="56"/>
+      <c r="E8" s="81" t="s">
         <v>2</v>
       </c>
-      <c r="F8" s="75"/>
-      <c r="G8" s="75"/>
-      <c r="H8" s="75" t="s">
+      <c r="F8" s="82"/>
+      <c r="G8" s="82"/>
+      <c r="H8" s="82" t="s">
         <v>4</v>
       </c>
-      <c r="I8" s="75"/>
-      <c r="J8" s="75"/>
-      <c r="K8" s="75"/>
-      <c r="L8" s="75"/>
-      <c r="M8" s="75"/>
-      <c r="N8" s="76"/>
-      <c r="O8" s="77"/>
+      <c r="I8" s="82"/>
+      <c r="J8" s="82"/>
+      <c r="K8" s="82"/>
+      <c r="L8" s="82"/>
+      <c r="M8" s="82"/>
+      <c r="N8" s="83"/>
+      <c r="O8" s="84"/>
     </row>
     <row r="9" spans="2:15" ht="40.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="95"/>
-      <c r="C9" s="96"/>
-      <c r="D9" s="97"/>
-      <c r="E9" s="78" t="s">
+      <c r="B9" s="57"/>
+      <c r="C9" s="58"/>
+      <c r="D9" s="59"/>
+      <c r="E9" s="85" t="s">
         <v>48</v>
       </c>
-      <c r="F9" s="79"/>
-      <c r="G9" s="79"/>
-      <c r="H9" s="37" t="s">
+      <c r="F9" s="86"/>
+      <c r="G9" s="86"/>
+      <c r="H9" s="99" t="s">
         <v>49</v>
       </c>
-      <c r="I9" s="37"/>
-      <c r="J9" s="37"/>
-      <c r="K9" s="37"/>
-      <c r="L9" s="37"/>
-      <c r="M9" s="37"/>
-      <c r="N9" s="38"/>
-      <c r="O9" s="39"/>
+      <c r="I9" s="99"/>
+      <c r="J9" s="99"/>
+      <c r="K9" s="99"/>
+      <c r="L9" s="99"/>
+      <c r="M9" s="99"/>
+      <c r="N9" s="100"/>
+      <c r="O9" s="101"/>
     </row>
     <row r="10" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="11" spans="2:15" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="101" t="s">
+      <c r="B11" s="90" t="s">
         <v>18</v>
       </c>
-      <c r="C11" s="102"/>
-      <c r="D11" s="102"/>
-      <c r="E11" s="102"/>
-      <c r="F11" s="102"/>
-      <c r="G11" s="102"/>
-      <c r="H11" s="102"/>
-      <c r="I11" s="102"/>
-      <c r="J11" s="102"/>
-      <c r="K11" s="102"/>
-      <c r="L11" s="102"/>
-      <c r="M11" s="102"/>
-      <c r="N11" s="102"/>
-      <c r="O11" s="103"/>
+      <c r="C11" s="91"/>
+      <c r="D11" s="91"/>
+      <c r="E11" s="91"/>
+      <c r="F11" s="91"/>
+      <c r="G11" s="91"/>
+      <c r="H11" s="91"/>
+      <c r="I11" s="91"/>
+      <c r="J11" s="91"/>
+      <c r="K11" s="91"/>
+      <c r="L11" s="91"/>
+      <c r="M11" s="91"/>
+      <c r="N11" s="91"/>
+      <c r="O11" s="92"/>
     </row>
     <row r="12" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="13" spans="2:15" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="104" t="s">
+      <c r="B13" s="113" t="s">
         <v>5</v>
       </c>
-      <c r="C13" s="105"/>
-      <c r="D13" s="105"/>
-      <c r="E13" s="105"/>
-      <c r="F13" s="105"/>
-      <c r="G13" s="105"/>
-      <c r="H13" s="106"/>
+      <c r="C13" s="114"/>
+      <c r="D13" s="114"/>
+      <c r="E13" s="114"/>
+      <c r="F13" s="114"/>
+      <c r="G13" s="114"/>
+      <c r="H13" s="115"/>
       <c r="I13" s="2"/>
-      <c r="J13" s="58" t="s">
+      <c r="J13" s="68" t="s">
         <v>19</v>
       </c>
-      <c r="K13" s="59"/>
-      <c r="L13" s="59"/>
-      <c r="M13" s="59"/>
-      <c r="N13" s="60"/>
-      <c r="O13" s="61"/>
+      <c r="K13" s="69"/>
+      <c r="L13" s="69"/>
+      <c r="M13" s="69"/>
+      <c r="N13" s="70"/>
+      <c r="O13" s="71"/>
     </row>
     <row r="14" spans="2:15" ht="31.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="107" t="s">
+      <c r="B14" s="116" t="s">
         <v>6</v>
       </c>
-      <c r="C14" s="68"/>
-      <c r="D14" s="68"/>
-      <c r="E14" s="68" t="s">
+      <c r="C14" s="75"/>
+      <c r="D14" s="75"/>
+      <c r="E14" s="75" t="s">
         <v>35</v>
       </c>
-      <c r="F14" s="68"/>
-      <c r="G14" s="68" t="s">
+      <c r="F14" s="75"/>
+      <c r="G14" s="75" t="s">
         <v>7</v>
       </c>
-      <c r="H14" s="69"/>
+      <c r="H14" s="76"/>
       <c r="I14" s="3"/>
       <c r="J14" s="19" t="s">
         <v>0</v>
@@ -2190,19 +2190,19 @@
       </c>
     </row>
     <row r="15" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="108" t="s">
+      <c r="B15" s="117" t="s">
         <v>8</v>
       </c>
-      <c r="C15" s="64"/>
-      <c r="D15" s="64"/>
-      <c r="E15" s="64">
-        <v>0</v>
-      </c>
-      <c r="F15" s="64"/>
-      <c r="G15" s="48">
-        <v>0</v>
-      </c>
-      <c r="H15" s="49"/>
+      <c r="C15" s="74"/>
+      <c r="D15" s="74"/>
+      <c r="E15" s="74">
+        <v>0</v>
+      </c>
+      <c r="F15" s="74"/>
+      <c r="G15" s="34">
+        <v>0</v>
+      </c>
+      <c r="H15" s="35"/>
       <c r="I15" s="1"/>
       <c r="J15" s="18" t="s">
         <v>11</v>
@@ -2224,19 +2224,19 @@
       </c>
     </row>
     <row r="16" spans="2:15" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="B16" s="109" t="s">
+      <c r="B16" s="39" t="s">
         <v>9</v>
       </c>
-      <c r="C16" s="110"/>
-      <c r="D16" s="111"/>
-      <c r="E16" s="64">
-        <v>0</v>
-      </c>
-      <c r="F16" s="64"/>
-      <c r="G16" s="48">
-        <v>0</v>
-      </c>
-      <c r="H16" s="49"/>
+      <c r="C16" s="40"/>
+      <c r="D16" s="41"/>
+      <c r="E16" s="74">
+        <v>0</v>
+      </c>
+      <c r="F16" s="74"/>
+      <c r="G16" s="34">
+        <v>0</v>
+      </c>
+      <c r="H16" s="35"/>
       <c r="I16" s="1"/>
       <c r="J16" s="17" t="s">
         <v>42</v>
@@ -2263,19 +2263,19 @@
       </c>
     </row>
     <row r="17" spans="2:15" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="116" t="s">
+      <c r="B17" s="36" t="s">
         <v>34</v>
       </c>
-      <c r="C17" s="117"/>
-      <c r="D17" s="118"/>
-      <c r="E17" s="47" t="s">
+      <c r="C17" s="37"/>
+      <c r="D17" s="38"/>
+      <c r="E17" s="109" t="s">
         <v>36</v>
       </c>
-      <c r="F17" s="47"/>
-      <c r="G17" s="48">
-        <v>0</v>
-      </c>
-      <c r="H17" s="49"/>
+      <c r="F17" s="109"/>
+      <c r="G17" s="34">
+        <v>0</v>
+      </c>
+      <c r="H17" s="35"/>
       <c r="I17" s="1"/>
       <c r="J17" s="8" t="s">
         <v>33</v>
@@ -2297,19 +2297,19 @@
       </c>
     </row>
     <row r="18" spans="2:15" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="B18" s="109" t="s">
+      <c r="B18" s="39" t="s">
         <v>37</v>
       </c>
-      <c r="C18" s="110"/>
-      <c r="D18" s="111"/>
-      <c r="E18" s="64" t="s">
+      <c r="C18" s="40"/>
+      <c r="D18" s="41"/>
+      <c r="E18" s="74" t="s">
         <v>17</v>
       </c>
-      <c r="F18" s="64"/>
-      <c r="G18" s="48">
-        <v>0</v>
-      </c>
-      <c r="H18" s="49"/>
+      <c r="F18" s="74"/>
+      <c r="G18" s="34">
+        <v>0</v>
+      </c>
+      <c r="H18" s="35"/>
       <c r="I18" s="1"/>
       <c r="J18" s="8" t="s">
         <v>45</v>
@@ -2331,18 +2331,18 @@
       </c>
     </row>
     <row r="19" spans="2:15" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="98" t="s">
+      <c r="B19" s="87" t="s">
         <v>10</v>
       </c>
-      <c r="C19" s="99"/>
-      <c r="D19" s="99"/>
-      <c r="E19" s="99"/>
-      <c r="F19" s="100"/>
-      <c r="G19" s="62">
+      <c r="C19" s="88"/>
+      <c r="D19" s="88"/>
+      <c r="E19" s="88"/>
+      <c r="F19" s="89"/>
+      <c r="G19" s="72">
         <f>SUM(G15:H18)</f>
         <v>0</v>
       </c>
-      <c r="H19" s="63"/>
+      <c r="H19" s="73"/>
       <c r="I19" s="1"/>
       <c r="J19" s="23" t="s">
         <v>38</v>
@@ -2371,70 +2371,70 @@
       <c r="G20" s="1"/>
       <c r="H20" s="1"/>
       <c r="I20" s="1"/>
-      <c r="J20" s="65" t="s">
+      <c r="J20" s="110" t="s">
         <v>44</v>
       </c>
-      <c r="K20" s="66"/>
-      <c r="L20" s="66"/>
-      <c r="M20" s="66"/>
-      <c r="N20" s="66"/>
-      <c r="O20" s="67"/>
+      <c r="K20" s="111"/>
+      <c r="L20" s="111"/>
+      <c r="M20" s="111"/>
+      <c r="N20" s="111"/>
+      <c r="O20" s="112"/>
     </row>
     <row r="21" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="22" spans="2:15" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="101" t="s">
+      <c r="B22" s="90" t="s">
         <v>20</v>
       </c>
-      <c r="C22" s="102"/>
-      <c r="D22" s="102"/>
-      <c r="E22" s="102"/>
-      <c r="F22" s="102"/>
-      <c r="G22" s="102"/>
-      <c r="H22" s="102"/>
-      <c r="I22" s="102"/>
-      <c r="J22" s="102"/>
-      <c r="K22" s="102"/>
-      <c r="L22" s="102"/>
-      <c r="M22" s="102"/>
-      <c r="N22" s="102"/>
-      <c r="O22" s="103"/>
+      <c r="C22" s="91"/>
+      <c r="D22" s="91"/>
+      <c r="E22" s="91"/>
+      <c r="F22" s="91"/>
+      <c r="G22" s="91"/>
+      <c r="H22" s="91"/>
+      <c r="I22" s="91"/>
+      <c r="J22" s="91"/>
+      <c r="K22" s="91"/>
+      <c r="L22" s="91"/>
+      <c r="M22" s="91"/>
+      <c r="N22" s="91"/>
+      <c r="O22" s="92"/>
     </row>
     <row r="23" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="24" spans="2:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="101" t="s">
+      <c r="B24" s="90" t="s">
         <v>21</v>
       </c>
-      <c r="C24" s="102"/>
-      <c r="D24" s="102"/>
-      <c r="E24" s="102"/>
-      <c r="F24" s="102"/>
-      <c r="G24" s="102"/>
-      <c r="H24" s="102"/>
-      <c r="I24" s="103"/>
-      <c r="K24" s="112" t="s">
+      <c r="C24" s="91"/>
+      <c r="D24" s="91"/>
+      <c r="E24" s="91"/>
+      <c r="F24" s="91"/>
+      <c r="G24" s="91"/>
+      <c r="H24" s="91"/>
+      <c r="I24" s="92"/>
+      <c r="K24" s="118" t="s">
         <v>22</v>
       </c>
-      <c r="L24" s="113"/>
-      <c r="M24" s="113"/>
-      <c r="N24" s="114"/>
-      <c r="O24" s="115"/>
+      <c r="L24" s="119"/>
+      <c r="M24" s="119"/>
+      <c r="N24" s="120"/>
+      <c r="O24" s="121"/>
     </row>
     <row r="25" spans="2:15" ht="1.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="119"/>
-      <c r="C25" s="120"/>
-      <c r="D25" s="120"/>
-      <c r="E25" s="120"/>
-      <c r="F25" s="120"/>
-      <c r="G25" s="120"/>
-      <c r="H25" s="120"/>
-      <c r="I25" s="121"/>
-      <c r="K25" s="31" t="s">
+      <c r="B25" s="31"/>
+      <c r="C25" s="32"/>
+      <c r="D25" s="32"/>
+      <c r="E25" s="32"/>
+      <c r="F25" s="32"/>
+      <c r="G25" s="32"/>
+      <c r="H25" s="32"/>
+      <c r="I25" s="33"/>
+      <c r="K25" s="93" t="s">
         <v>23</v>
       </c>
-      <c r="L25" s="32"/>
-      <c r="M25" s="32"/>
-      <c r="N25" s="32"/>
-      <c r="O25" s="33"/>
+      <c r="L25" s="94"/>
+      <c r="M25" s="94"/>
+      <c r="N25" s="94"/>
+      <c r="O25" s="95"/>
     </row>
     <row r="26" spans="2:15" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B26" s="11"/>
@@ -2445,11 +2445,11 @@
       <c r="G26" s="5"/>
       <c r="H26" s="5"/>
       <c r="I26" s="12"/>
-      <c r="K26" s="34"/>
-      <c r="L26" s="35"/>
-      <c r="M26" s="35"/>
-      <c r="N26" s="35"/>
-      <c r="O26" s="36"/>
+      <c r="K26" s="96"/>
+      <c r="L26" s="97"/>
+      <c r="M26" s="97"/>
+      <c r="N26" s="97"/>
+      <c r="O26" s="98"/>
     </row>
     <row r="27" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B27" s="11"/>
@@ -2633,6 +2633,30 @@
     </row>
   </sheetData>
   <mergeCells count="40">
+    <mergeCell ref="J6:K6"/>
+    <mergeCell ref="L6:O6"/>
+    <mergeCell ref="E6:I6"/>
+    <mergeCell ref="E17:F17"/>
+    <mergeCell ref="G17:H17"/>
+    <mergeCell ref="B13:H13"/>
+    <mergeCell ref="B14:D14"/>
+    <mergeCell ref="B15:D15"/>
+    <mergeCell ref="B16:D16"/>
+    <mergeCell ref="E9:G9"/>
+    <mergeCell ref="B19:F19"/>
+    <mergeCell ref="B11:O11"/>
+    <mergeCell ref="K25:O26"/>
+    <mergeCell ref="H9:O9"/>
+    <mergeCell ref="J20:O20"/>
+    <mergeCell ref="B22:O22"/>
+    <mergeCell ref="B24:I24"/>
+    <mergeCell ref="K24:O24"/>
+    <mergeCell ref="E18:F18"/>
+    <mergeCell ref="G19:H19"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="G15:H15"/>
+    <mergeCell ref="G16:H16"/>
     <mergeCell ref="G18:H18"/>
     <mergeCell ref="B17:D17"/>
     <mergeCell ref="B18:D18"/>
@@ -2644,35 +2668,11 @@
     <mergeCell ref="E2:O2"/>
     <mergeCell ref="E5:O5"/>
     <mergeCell ref="J13:O13"/>
-    <mergeCell ref="G19:H19"/>
-    <mergeCell ref="E15:F15"/>
-    <mergeCell ref="E16:F16"/>
-    <mergeCell ref="G15:H15"/>
-    <mergeCell ref="G16:H16"/>
     <mergeCell ref="E14:F14"/>
     <mergeCell ref="G14:H14"/>
     <mergeCell ref="E4:O4"/>
     <mergeCell ref="E8:G8"/>
     <mergeCell ref="H8:O8"/>
-    <mergeCell ref="E9:G9"/>
-    <mergeCell ref="B19:F19"/>
-    <mergeCell ref="B11:O11"/>
-    <mergeCell ref="K25:O26"/>
-    <mergeCell ref="H9:O9"/>
-    <mergeCell ref="J6:K6"/>
-    <mergeCell ref="L6:O6"/>
-    <mergeCell ref="E6:I6"/>
-    <mergeCell ref="E17:F17"/>
-    <mergeCell ref="G17:H17"/>
-    <mergeCell ref="J20:O20"/>
-    <mergeCell ref="B22:O22"/>
-    <mergeCell ref="B24:I24"/>
-    <mergeCell ref="B13:H13"/>
-    <mergeCell ref="B14:D14"/>
-    <mergeCell ref="B15:D15"/>
-    <mergeCell ref="B16:D16"/>
-    <mergeCell ref="K24:O24"/>
-    <mergeCell ref="E18:F18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="57" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
updated transition reports bar charts
git-svn-id: svn://107.170.10.188:8080/Semoss/trunk@3029 ef391c1c-ee15-45f7-b1d6-dde3d27a2169

Former-commit-id: 5ec207ce40fc380c8bcd660645c5098228672f69
</commit_message>
<xml_diff>
--- a/export/Reports/TAP_Legacy_System_Dispositions_Template.xlsx
+++ b/export/Reports/TAP_Legacy_System_Dispositions_Template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mahkhalil\workspace\Semoss\export\Reports\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ksmart\workspace64bitNew\SEMOSS_2014\export\Reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -22,9 +22,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="53">
   <si>
-    <t>ABACUS</t>
-  </si>
-  <si>
     <t>System Description</t>
   </si>
   <si>
@@ -89,9 +86,6 @@
   </si>
   <si>
     <t>Interfaces Summary</t>
-  </si>
-  <si>
-    <t>The following graph illustrates the number of interfaces ABACUS will have in the future state based upon the business rules established for each interface type.</t>
   </si>
   <si>
     <t>Interface Type</t>
@@ -185,6 +179,12 @@
 4. Interface Modernization activities involve upgrading the legacy system to be able to exchange data with COTS EHR solution via SOA services and it is assumed that these activities must be completed before the COTS EHR solution is fielded for testing.
 5. Required interfaces are specified for LPI systems and are included in the interface modernization costs.
 6. Proposed interfaces are specified for LPNI systems and are included in the interface modernization costs.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> @SYSTEM@</t>
+  </si>
+  <si>
+    <t>The following graph illustrates the number of interfaces @SYSTEM@ will have in the future state based upon the business rules established for each interface type.</t>
   </si>
 </sst>
 </file>
@@ -1086,9 +1086,6 @@
     <xf numFmtId="0" fontId="10" fillId="6" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1128,6 +1125,171 @@
     <xf numFmtId="44" fontId="8" fillId="7" borderId="47" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="44" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="7" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="7" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="7" fillId="0" borderId="33" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="7" fillId="0" borderId="34" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1221,9 +1383,6 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1251,15 +1410,6 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1296,158 +1446,8 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="7" fillId="0" borderId="33" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="7" fillId="0" borderId="34" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="7" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="7" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="5" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="44" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1666,11 +1666,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="457780744"/>
-        <c:axId val="457781136"/>
+        <c:axId val="439276592"/>
+        <c:axId val="439276984"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="457780744"/>
+        <c:axId val="439276592"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1679,7 +1679,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="457781136"/>
+        <c:crossAx val="439276984"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1687,7 +1687,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="457781136"/>
+        <c:axId val="439276984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1698,7 +1698,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="457780744"/>
+        <c:crossAx val="439276592"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2064,8 +2064,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="B1:O46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="G49" sqref="G49"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2083,453 +2083,453 @@
   <sheetData>
     <row r="1" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:15" ht="72" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="79" t="s">
-        <v>31</v>
-      </c>
-      <c r="C2" s="80"/>
-      <c r="D2" s="81"/>
-      <c r="E2" s="54" t="s">
-        <v>32</v>
-      </c>
-      <c r="F2" s="55"/>
-      <c r="G2" s="55"/>
-      <c r="H2" s="55"/>
-      <c r="I2" s="55"/>
-      <c r="J2" s="55"/>
-      <c r="K2" s="55"/>
-      <c r="L2" s="55"/>
-      <c r="M2" s="55"/>
-      <c r="N2" s="56"/>
-      <c r="O2" s="57"/>
+      <c r="B2" s="129" t="s">
+        <v>29</v>
+      </c>
+      <c r="C2" s="130"/>
+      <c r="D2" s="131"/>
+      <c r="E2" s="108" t="s">
+        <v>30</v>
+      </c>
+      <c r="F2" s="109"/>
+      <c r="G2" s="109"/>
+      <c r="H2" s="109"/>
+      <c r="I2" s="109"/>
+      <c r="J2" s="109"/>
+      <c r="K2" s="109"/>
+      <c r="L2" s="109"/>
+      <c r="M2" s="109"/>
+      <c r="N2" s="110"/>
+      <c r="O2" s="111"/>
     </row>
     <row r="3" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="2:15" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="82" t="s">
-        <v>46</v>
-      </c>
-      <c r="C4" s="83"/>
-      <c r="D4" s="84"/>
-      <c r="E4" s="68" t="s">
-        <v>1</v>
-      </c>
-      <c r="F4" s="69"/>
-      <c r="G4" s="69"/>
-      <c r="H4" s="69"/>
-      <c r="I4" s="69"/>
-      <c r="J4" s="69"/>
-      <c r="K4" s="69"/>
-      <c r="L4" s="69"/>
-      <c r="M4" s="69"/>
-      <c r="N4" s="70"/>
-      <c r="O4" s="71"/>
+      <c r="B4" s="132" t="s">
+        <v>44</v>
+      </c>
+      <c r="C4" s="133"/>
+      <c r="D4" s="134"/>
+      <c r="E4" s="121" t="s">
+        <v>0</v>
+      </c>
+      <c r="F4" s="122"/>
+      <c r="G4" s="122"/>
+      <c r="H4" s="122"/>
+      <c r="I4" s="122"/>
+      <c r="J4" s="122"/>
+      <c r="K4" s="122"/>
+      <c r="L4" s="122"/>
+      <c r="M4" s="122"/>
+      <c r="N4" s="123"/>
+      <c r="O4" s="124"/>
     </row>
     <row r="5" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="85" t="s">
+      <c r="B5" s="135" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="136"/>
+      <c r="D5" s="137"/>
+      <c r="E5" s="112" t="s">
+        <v>45</v>
+      </c>
+      <c r="F5" s="113"/>
+      <c r="G5" s="113"/>
+      <c r="H5" s="113"/>
+      <c r="I5" s="113"/>
+      <c r="J5" s="113"/>
+      <c r="K5" s="113"/>
+      <c r="L5" s="113"/>
+      <c r="M5" s="113"/>
+      <c r="N5" s="114"/>
+      <c r="O5" s="115"/>
+    </row>
+    <row r="6" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="138" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="86"/>
-      <c r="D5" s="87"/>
-      <c r="E5" s="58" t="s">
-        <v>47</v>
-      </c>
-      <c r="F5" s="59"/>
-      <c r="G5" s="59"/>
-      <c r="H5" s="59"/>
-      <c r="I5" s="59"/>
-      <c r="J5" s="59"/>
-      <c r="K5" s="59"/>
-      <c r="L5" s="59"/>
-      <c r="M5" s="59"/>
-      <c r="N5" s="60"/>
-      <c r="O5" s="61"/>
-    </row>
-    <row r="6" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="88" t="s">
-        <v>16</v>
-      </c>
-      <c r="C6" s="89"/>
-      <c r="D6" s="90"/>
-      <c r="E6" s="132">
+      <c r="C6" s="139"/>
+      <c r="D6" s="140"/>
+      <c r="E6" s="42">
         <v>42005</v>
       </c>
-      <c r="F6" s="133"/>
-      <c r="G6" s="133"/>
-      <c r="H6" s="133"/>
-      <c r="I6" s="133"/>
-      <c r="J6" s="127" t="s">
-        <v>40</v>
-      </c>
-      <c r="K6" s="127"/>
-      <c r="L6" s="128">
+      <c r="F6" s="43"/>
+      <c r="G6" s="43"/>
+      <c r="H6" s="43"/>
+      <c r="I6" s="43"/>
+      <c r="J6" s="37" t="s">
+        <v>38</v>
+      </c>
+      <c r="K6" s="37"/>
+      <c r="L6" s="38">
         <v>42005</v>
       </c>
-      <c r="M6" s="129"/>
-      <c r="N6" s="130"/>
-      <c r="O6" s="131"/>
+      <c r="M6" s="39"/>
+      <c r="N6" s="40"/>
+      <c r="O6" s="41"/>
     </row>
     <row r="7" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="8" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="91" t="s">
+      <c r="B8" s="59" t="s">
+        <v>2</v>
+      </c>
+      <c r="C8" s="60"/>
+      <c r="D8" s="61"/>
+      <c r="E8" s="125" t="s">
+        <v>1</v>
+      </c>
+      <c r="F8" s="126"/>
+      <c r="G8" s="126"/>
+      <c r="H8" s="126" t="s">
         <v>3</v>
       </c>
-      <c r="C8" s="92"/>
-      <c r="D8" s="93"/>
-      <c r="E8" s="72" t="s">
-        <v>2</v>
-      </c>
-      <c r="F8" s="73"/>
-      <c r="G8" s="73"/>
-      <c r="H8" s="73" t="s">
-        <v>4</v>
-      </c>
-      <c r="I8" s="73"/>
-      <c r="J8" s="73"/>
-      <c r="K8" s="73"/>
-      <c r="L8" s="73"/>
-      <c r="M8" s="73"/>
-      <c r="N8" s="74"/>
-      <c r="O8" s="75"/>
+      <c r="I8" s="126"/>
+      <c r="J8" s="126"/>
+      <c r="K8" s="126"/>
+      <c r="L8" s="126"/>
+      <c r="M8" s="126"/>
+      <c r="N8" s="127"/>
+      <c r="O8" s="128"/>
     </row>
     <row r="9" spans="2:15" ht="40.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="94"/>
-      <c r="C9" s="95"/>
-      <c r="D9" s="96"/>
-      <c r="E9" s="140" t="s">
-        <v>48</v>
-      </c>
-      <c r="F9" s="141"/>
-      <c r="G9" s="141"/>
-      <c r="H9" s="109" t="s">
-        <v>49</v>
-      </c>
-      <c r="I9" s="109"/>
-      <c r="J9" s="109"/>
-      <c r="K9" s="109"/>
-      <c r="L9" s="109"/>
-      <c r="M9" s="109"/>
-      <c r="N9" s="110"/>
-      <c r="O9" s="111"/>
+      <c r="B9" s="62"/>
+      <c r="C9" s="63"/>
+      <c r="D9" s="64"/>
+      <c r="E9" s="57" t="s">
+        <v>46</v>
+      </c>
+      <c r="F9" s="58"/>
+      <c r="G9" s="58"/>
+      <c r="H9" s="77" t="s">
+        <v>47</v>
+      </c>
+      <c r="I9" s="77"/>
+      <c r="J9" s="77"/>
+      <c r="K9" s="77"/>
+      <c r="L9" s="77"/>
+      <c r="M9" s="77"/>
+      <c r="N9" s="78"/>
+      <c r="O9" s="79"/>
     </row>
     <row r="10" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="11" spans="2:15" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="100" t="s">
-        <v>18</v>
-      </c>
-      <c r="C11" s="101"/>
-      <c r="D11" s="101"/>
-      <c r="E11" s="101"/>
-      <c r="F11" s="101"/>
-      <c r="G11" s="101"/>
-      <c r="H11" s="101"/>
-      <c r="I11" s="101"/>
-      <c r="J11" s="101"/>
-      <c r="K11" s="101"/>
-      <c r="L11" s="101"/>
-      <c r="M11" s="101"/>
-      <c r="N11" s="101"/>
-      <c r="O11" s="102"/>
+      <c r="B11" s="68" t="s">
+        <v>17</v>
+      </c>
+      <c r="C11" s="69"/>
+      <c r="D11" s="69"/>
+      <c r="E11" s="69"/>
+      <c r="F11" s="69"/>
+      <c r="G11" s="69"/>
+      <c r="H11" s="69"/>
+      <c r="I11" s="69"/>
+      <c r="J11" s="69"/>
+      <c r="K11" s="69"/>
+      <c r="L11" s="69"/>
+      <c r="M11" s="69"/>
+      <c r="N11" s="69"/>
+      <c r="O11" s="70"/>
     </row>
     <row r="12" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="13" spans="2:15" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="135" t="s">
+      <c r="B13" s="47" t="s">
+        <v>4</v>
+      </c>
+      <c r="C13" s="48"/>
+      <c r="D13" s="48"/>
+      <c r="E13" s="48"/>
+      <c r="F13" s="48"/>
+      <c r="G13" s="48"/>
+      <c r="H13" s="49"/>
+      <c r="I13" s="2"/>
+      <c r="J13" s="116" t="s">
+        <v>18</v>
+      </c>
+      <c r="K13" s="117"/>
+      <c r="L13" s="117"/>
+      <c r="M13" s="117"/>
+      <c r="N13" s="118"/>
+      <c r="O13" s="119"/>
+    </row>
+    <row r="14" spans="2:15" ht="31.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B14" s="50" t="s">
         <v>5</v>
       </c>
-      <c r="C13" s="136"/>
-      <c r="D13" s="136"/>
-      <c r="E13" s="136"/>
-      <c r="F13" s="136"/>
-      <c r="G13" s="136"/>
-      <c r="H13" s="137"/>
-      <c r="I13" s="2"/>
-      <c r="J13" s="62" t="s">
-        <v>19</v>
-      </c>
-      <c r="K13" s="63"/>
-      <c r="L13" s="63"/>
-      <c r="M13" s="63"/>
-      <c r="N13" s="64"/>
-      <c r="O13" s="65"/>
-    </row>
-    <row r="14" spans="2:15" ht="31.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="138" t="s">
+      <c r="C14" s="51"/>
+      <c r="D14" s="51"/>
+      <c r="E14" s="51" t="s">
+        <v>33</v>
+      </c>
+      <c r="F14" s="51"/>
+      <c r="G14" s="51" t="s">
         <v>6</v>
       </c>
-      <c r="C14" s="66"/>
-      <c r="D14" s="66"/>
-      <c r="E14" s="66" t="s">
-        <v>35</v>
-      </c>
-      <c r="F14" s="66"/>
-      <c r="G14" s="66" t="s">
+      <c r="H14" s="120"/>
+      <c r="I14" s="3"/>
+      <c r="J14" s="141" t="s">
+        <v>51</v>
+      </c>
+      <c r="K14" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="L14" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="M14" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="N14" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="O14" s="20" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="15" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B15" s="52" t="s">
         <v>7</v>
       </c>
-      <c r="H14" s="67"/>
-      <c r="I14" s="3"/>
-      <c r="J14" s="19" t="s">
-        <v>0</v>
-      </c>
-      <c r="K14" s="20" t="s">
-        <v>39</v>
-      </c>
-      <c r="L14" s="20" t="s">
-        <v>12</v>
-      </c>
-      <c r="M14" s="20" t="s">
-        <v>13</v>
-      </c>
-      <c r="N14" s="20" t="s">
-        <v>14</v>
-      </c>
-      <c r="O14" s="21" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="15" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="139" t="s">
-        <v>8</v>
-      </c>
-      <c r="C15" s="119"/>
-      <c r="D15" s="119"/>
-      <c r="E15" s="119">
-        <v>0</v>
-      </c>
-      <c r="F15" s="119"/>
-      <c r="G15" s="122">
-        <v>0</v>
-      </c>
-      <c r="H15" s="123"/>
+      <c r="C15" s="53"/>
+      <c r="D15" s="53"/>
+      <c r="E15" s="53">
+        <v>0</v>
+      </c>
+      <c r="F15" s="53"/>
+      <c r="G15" s="45">
+        <v>0</v>
+      </c>
+      <c r="H15" s="46"/>
       <c r="I15" s="1"/>
       <c r="J15" s="18" t="s">
-        <v>11</v>
-      </c>
-      <c r="K15" s="24">
-        <v>0</v>
-      </c>
-      <c r="L15" s="24">
-        <v>0</v>
-      </c>
-      <c r="M15" s="24">
-        <v>0</v>
-      </c>
-      <c r="N15" s="24">
-        <v>0</v>
-      </c>
-      <c r="O15" s="25">
+        <v>10</v>
+      </c>
+      <c r="K15" s="23">
+        <v>0</v>
+      </c>
+      <c r="L15" s="23">
+        <v>0</v>
+      </c>
+      <c r="M15" s="23">
+        <v>0</v>
+      </c>
+      <c r="N15" s="23">
+        <v>0</v>
+      </c>
+      <c r="O15" s="24">
         <v>0</v>
       </c>
     </row>
     <row r="16" spans="2:15" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="B16" s="76" t="s">
-        <v>9</v>
-      </c>
-      <c r="C16" s="77"/>
-      <c r="D16" s="78"/>
-      <c r="E16" s="119">
-        <v>0</v>
-      </c>
-      <c r="F16" s="119"/>
-      <c r="G16" s="122">
-        <v>0</v>
-      </c>
-      <c r="H16" s="123"/>
+      <c r="B16" s="54" t="s">
+        <v>8</v>
+      </c>
+      <c r="C16" s="55"/>
+      <c r="D16" s="56"/>
+      <c r="E16" s="53">
+        <v>0</v>
+      </c>
+      <c r="F16" s="53"/>
+      <c r="G16" s="45">
+        <v>0</v>
+      </c>
+      <c r="H16" s="46"/>
       <c r="I16" s="1"/>
       <c r="J16" s="17" t="s">
-        <v>42</v>
-      </c>
-      <c r="K16" s="26">
+        <v>40</v>
+      </c>
+      <c r="K16" s="25">
         <f>SUM(K17:K19)</f>
         <v>0</v>
       </c>
-      <c r="L16" s="26">
+      <c r="L16" s="25">
         <f>SUM(L17:L19)</f>
         <v>0</v>
       </c>
-      <c r="M16" s="26">
+      <c r="M16" s="25">
         <f>SUM(M17:M19)</f>
         <v>0</v>
       </c>
-      <c r="N16" s="26">
+      <c r="N16" s="25">
         <f>SUM(N17:N19)</f>
         <v>0</v>
       </c>
-      <c r="O16" s="34">
+      <c r="O16" s="33">
         <f>SUM(O17:O19)</f>
         <v>0</v>
       </c>
     </row>
     <row r="17" spans="2:15" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="124" t="s">
+      <c r="B17" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="C17" s="35"/>
+      <c r="D17" s="36"/>
+      <c r="E17" s="44" t="s">
         <v>34</v>
       </c>
-      <c r="C17" s="125"/>
-      <c r="D17" s="126"/>
-      <c r="E17" s="134" t="s">
-        <v>36</v>
-      </c>
-      <c r="F17" s="134"/>
-      <c r="G17" s="122">
-        <v>0</v>
-      </c>
-      <c r="H17" s="123"/>
+      <c r="F17" s="44"/>
+      <c r="G17" s="45">
+        <v>0</v>
+      </c>
+      <c r="H17" s="46"/>
       <c r="I17" s="1"/>
       <c r="J17" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="K17" s="27">
-        <v>0</v>
-      </c>
-      <c r="L17" s="27">
-        <v>0</v>
-      </c>
-      <c r="M17" s="27">
-        <v>0</v>
-      </c>
-      <c r="N17" s="27">
-        <v>0</v>
-      </c>
-      <c r="O17" s="28">
+        <v>31</v>
+      </c>
+      <c r="K17" s="26">
+        <v>0</v>
+      </c>
+      <c r="L17" s="26">
+        <v>0</v>
+      </c>
+      <c r="M17" s="26">
+        <v>0</v>
+      </c>
+      <c r="N17" s="26">
+        <v>0</v>
+      </c>
+      <c r="O17" s="27">
         <v>0</v>
       </c>
     </row>
     <row r="18" spans="2:15" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="B18" s="76" t="s">
-        <v>37</v>
-      </c>
-      <c r="C18" s="77"/>
-      <c r="D18" s="78"/>
-      <c r="E18" s="119" t="s">
-        <v>17</v>
-      </c>
-      <c r="F18" s="119"/>
-      <c r="G18" s="122">
-        <v>0</v>
-      </c>
-      <c r="H18" s="123"/>
+      <c r="B18" s="54" t="s">
+        <v>35</v>
+      </c>
+      <c r="C18" s="55"/>
+      <c r="D18" s="56"/>
+      <c r="E18" s="53" t="s">
+        <v>16</v>
+      </c>
+      <c r="F18" s="53"/>
+      <c r="G18" s="45">
+        <v>0</v>
+      </c>
+      <c r="H18" s="46"/>
       <c r="I18" s="1"/>
       <c r="J18" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="K18" s="27">
-        <v>0</v>
-      </c>
-      <c r="L18" s="27">
-        <v>0</v>
-      </c>
-      <c r="M18" s="27">
-        <v>0</v>
-      </c>
-      <c r="N18" s="27">
-        <v>0</v>
-      </c>
-      <c r="O18" s="28">
+        <v>43</v>
+      </c>
+      <c r="K18" s="26">
+        <v>0</v>
+      </c>
+      <c r="L18" s="26">
+        <v>0</v>
+      </c>
+      <c r="M18" s="26">
+        <v>0</v>
+      </c>
+      <c r="N18" s="26">
+        <v>0</v>
+      </c>
+      <c r="O18" s="27">
         <v>0</v>
       </c>
     </row>
     <row r="19" spans="2:15" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="97" t="s">
-        <v>10</v>
-      </c>
-      <c r="C19" s="98"/>
-      <c r="D19" s="98"/>
-      <c r="E19" s="98"/>
-      <c r="F19" s="99"/>
-      <c r="G19" s="120">
+      <c r="B19" s="65" t="s">
+        <v>9</v>
+      </c>
+      <c r="C19" s="66"/>
+      <c r="D19" s="66"/>
+      <c r="E19" s="66"/>
+      <c r="F19" s="67"/>
+      <c r="G19" s="87">
         <f>SUM(G15:H18)</f>
         <v>0</v>
       </c>
-      <c r="H19" s="121"/>
+      <c r="H19" s="88"/>
       <c r="I19" s="1"/>
-      <c r="J19" s="23" t="s">
-        <v>38</v>
-      </c>
-      <c r="K19" s="29">
-        <v>0</v>
-      </c>
-      <c r="L19" s="29">
-        <v>0</v>
-      </c>
-      <c r="M19" s="29">
-        <v>0</v>
-      </c>
-      <c r="N19" s="29">
-        <v>0</v>
-      </c>
-      <c r="O19" s="30">
+      <c r="J19" s="22" t="s">
+        <v>36</v>
+      </c>
+      <c r="K19" s="28">
+        <v>0</v>
+      </c>
+      <c r="L19" s="28">
+        <v>0</v>
+      </c>
+      <c r="M19" s="28">
+        <v>0</v>
+      </c>
+      <c r="N19" s="28">
+        <v>0</v>
+      </c>
+      <c r="O19" s="29">
         <v>0</v>
       </c>
     </row>
     <row r="20" spans="2:15" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C20" s="22"/>
-      <c r="D20" s="22"/>
-      <c r="E20" s="22"/>
-      <c r="F20" s="22"/>
+      <c r="C20" s="21"/>
+      <c r="D20" s="21"/>
+      <c r="E20" s="21"/>
+      <c r="F20" s="21"/>
       <c r="G20" s="1"/>
       <c r="H20" s="1"/>
       <c r="I20" s="1"/>
-      <c r="J20" s="112" t="s">
-        <v>44</v>
-      </c>
-      <c r="K20" s="113"/>
-      <c r="L20" s="113"/>
-      <c r="M20" s="113"/>
-      <c r="N20" s="113"/>
-      <c r="O20" s="114"/>
+      <c r="J20" s="80" t="s">
+        <v>42</v>
+      </c>
+      <c r="K20" s="81"/>
+      <c r="L20" s="81"/>
+      <c r="M20" s="81"/>
+      <c r="N20" s="81"/>
+      <c r="O20" s="82"/>
     </row>
     <row r="21" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="22" spans="2:15" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="100" t="s">
-        <v>20</v>
-      </c>
-      <c r="C22" s="101"/>
-      <c r="D22" s="101"/>
-      <c r="E22" s="101"/>
-      <c r="F22" s="101"/>
-      <c r="G22" s="101"/>
-      <c r="H22" s="101"/>
-      <c r="I22" s="101"/>
-      <c r="J22" s="101"/>
-      <c r="K22" s="101"/>
-      <c r="L22" s="101"/>
-      <c r="M22" s="101"/>
-      <c r="N22" s="101"/>
-      <c r="O22" s="102"/>
+      <c r="B22" s="68" t="s">
+        <v>19</v>
+      </c>
+      <c r="C22" s="69"/>
+      <c r="D22" s="69"/>
+      <c r="E22" s="69"/>
+      <c r="F22" s="69"/>
+      <c r="G22" s="69"/>
+      <c r="H22" s="69"/>
+      <c r="I22" s="69"/>
+      <c r="J22" s="69"/>
+      <c r="K22" s="69"/>
+      <c r="L22" s="69"/>
+      <c r="M22" s="69"/>
+      <c r="N22" s="69"/>
+      <c r="O22" s="70"/>
     </row>
     <row r="23" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="24" spans="2:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="100" t="s">
+      <c r="B24" s="68" t="s">
+        <v>20</v>
+      </c>
+      <c r="C24" s="69"/>
+      <c r="D24" s="69"/>
+      <c r="E24" s="69"/>
+      <c r="F24" s="69"/>
+      <c r="G24" s="69"/>
+      <c r="H24" s="69"/>
+      <c r="I24" s="70"/>
+      <c r="K24" s="83" t="s">
         <v>21</v>
       </c>
-      <c r="C24" s="101"/>
-      <c r="D24" s="101"/>
-      <c r="E24" s="101"/>
-      <c r="F24" s="101"/>
-      <c r="G24" s="101"/>
-      <c r="H24" s="101"/>
-      <c r="I24" s="102"/>
-      <c r="K24" s="115" t="s">
-        <v>22</v>
-      </c>
-      <c r="L24" s="116"/>
-      <c r="M24" s="116"/>
-      <c r="N24" s="117"/>
-      <c r="O24" s="118"/>
+      <c r="L24" s="84"/>
+      <c r="M24" s="84"/>
+      <c r="N24" s="85"/>
+      <c r="O24" s="86"/>
     </row>
     <row r="25" spans="2:15" ht="3" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="31"/>
-      <c r="C25" s="32"/>
-      <c r="D25" s="32"/>
-      <c r="E25" s="32"/>
-      <c r="F25" s="32"/>
-      <c r="G25" s="32"/>
-      <c r="H25" s="32"/>
-      <c r="I25" s="33"/>
-      <c r="K25" s="103" t="s">
-        <v>23</v>
-      </c>
-      <c r="L25" s="104"/>
-      <c r="M25" s="104"/>
-      <c r="N25" s="104"/>
-      <c r="O25" s="105"/>
+      <c r="B25" s="30"/>
+      <c r="C25" s="31"/>
+      <c r="D25" s="31"/>
+      <c r="E25" s="31"/>
+      <c r="F25" s="31"/>
+      <c r="G25" s="31"/>
+      <c r="H25" s="31"/>
+      <c r="I25" s="32"/>
+      <c r="K25" s="71" t="s">
+        <v>52</v>
+      </c>
+      <c r="L25" s="72"/>
+      <c r="M25" s="72"/>
+      <c r="N25" s="72"/>
+      <c r="O25" s="73"/>
     </row>
     <row r="26" spans="2:15" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B26" s="11"/>
@@ -2540,11 +2540,11 @@
       <c r="G26" s="5"/>
       <c r="H26" s="5"/>
       <c r="I26" s="12"/>
-      <c r="K26" s="106"/>
-      <c r="L26" s="107"/>
-      <c r="M26" s="107"/>
-      <c r="N26" s="107"/>
-      <c r="O26" s="108"/>
+      <c r="K26" s="74"/>
+      <c r="L26" s="75"/>
+      <c r="M26" s="75"/>
+      <c r="N26" s="75"/>
+      <c r="O26" s="76"/>
     </row>
     <row r="27" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B27" s="11"/>
@@ -2728,152 +2728,125 @@
     </row>
     <row r="39" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="40" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B40" s="45" t="s">
+      <c r="B40" s="99" t="s">
+        <v>48</v>
+      </c>
+      <c r="C40" s="100"/>
+      <c r="D40" s="101"/>
+      <c r="E40" s="89" t="s">
+        <v>49</v>
+      </c>
+      <c r="F40" s="90"/>
+      <c r="G40" s="90"/>
+      <c r="H40" s="90"/>
+      <c r="I40" s="90"/>
+      <c r="J40" s="90"/>
+      <c r="K40" s="90"/>
+      <c r="L40" s="90"/>
+      <c r="M40" s="90"/>
+      <c r="N40" s="90"/>
+      <c r="O40" s="91"/>
+    </row>
+    <row r="41" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B41" s="102"/>
+      <c r="C41" s="103"/>
+      <c r="D41" s="104"/>
+      <c r="E41" s="92" t="s">
         <v>50</v>
       </c>
-      <c r="C40" s="46"/>
-      <c r="D40" s="47"/>
-      <c r="E40" s="35" t="s">
-        <v>51</v>
-      </c>
-      <c r="F40" s="36"/>
-      <c r="G40" s="36"/>
-      <c r="H40" s="36"/>
-      <c r="I40" s="36"/>
-      <c r="J40" s="36"/>
-      <c r="K40" s="36"/>
-      <c r="L40" s="36"/>
-      <c r="M40" s="36"/>
-      <c r="N40" s="36"/>
-      <c r="O40" s="37"/>
-    </row>
-    <row r="41" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B41" s="48"/>
-      <c r="C41" s="49"/>
-      <c r="D41" s="50"/>
-      <c r="E41" s="38" t="s">
-        <v>52</v>
-      </c>
-      <c r="F41" s="39"/>
-      <c r="G41" s="39"/>
-      <c r="H41" s="39"/>
-      <c r="I41" s="39"/>
-      <c r="J41" s="39"/>
-      <c r="K41" s="39"/>
-      <c r="L41" s="39"/>
-      <c r="M41" s="39"/>
-      <c r="N41" s="39"/>
-      <c r="O41" s="40"/>
+      <c r="F41" s="93"/>
+      <c r="G41" s="93"/>
+      <c r="H41" s="93"/>
+      <c r="I41" s="93"/>
+      <c r="J41" s="93"/>
+      <c r="K41" s="93"/>
+      <c r="L41" s="93"/>
+      <c r="M41" s="93"/>
+      <c r="N41" s="93"/>
+      <c r="O41" s="94"/>
     </row>
     <row r="42" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B42" s="48"/>
-      <c r="C42" s="49"/>
-      <c r="D42" s="50"/>
-      <c r="E42" s="41"/>
-      <c r="F42" s="39"/>
-      <c r="G42" s="39"/>
-      <c r="H42" s="39"/>
-      <c r="I42" s="39"/>
-      <c r="J42" s="39"/>
-      <c r="K42" s="39"/>
-      <c r="L42" s="39"/>
-      <c r="M42" s="39"/>
-      <c r="N42" s="39"/>
-      <c r="O42" s="40"/>
+      <c r="B42" s="102"/>
+      <c r="C42" s="103"/>
+      <c r="D42" s="104"/>
+      <c r="E42" s="95"/>
+      <c r="F42" s="93"/>
+      <c r="G42" s="93"/>
+      <c r="H42" s="93"/>
+      <c r="I42" s="93"/>
+      <c r="J42" s="93"/>
+      <c r="K42" s="93"/>
+      <c r="L42" s="93"/>
+      <c r="M42" s="93"/>
+      <c r="N42" s="93"/>
+      <c r="O42" s="94"/>
     </row>
     <row r="43" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B43" s="48"/>
-      <c r="C43" s="49"/>
-      <c r="D43" s="50"/>
-      <c r="E43" s="41"/>
-      <c r="F43" s="39"/>
-      <c r="G43" s="39"/>
-      <c r="H43" s="39"/>
-      <c r="I43" s="39"/>
-      <c r="J43" s="39"/>
-      <c r="K43" s="39"/>
-      <c r="L43" s="39"/>
-      <c r="M43" s="39"/>
-      <c r="N43" s="39"/>
-      <c r="O43" s="40"/>
+      <c r="B43" s="102"/>
+      <c r="C43" s="103"/>
+      <c r="D43" s="104"/>
+      <c r="E43" s="95"/>
+      <c r="F43" s="93"/>
+      <c r="G43" s="93"/>
+      <c r="H43" s="93"/>
+      <c r="I43" s="93"/>
+      <c r="J43" s="93"/>
+      <c r="K43" s="93"/>
+      <c r="L43" s="93"/>
+      <c r="M43" s="93"/>
+      <c r="N43" s="93"/>
+      <c r="O43" s="94"/>
     </row>
     <row r="44" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B44" s="48"/>
-      <c r="C44" s="49"/>
-      <c r="D44" s="50"/>
-      <c r="E44" s="41"/>
-      <c r="F44" s="39"/>
-      <c r="G44" s="39"/>
-      <c r="H44" s="39"/>
-      <c r="I44" s="39"/>
-      <c r="J44" s="39"/>
-      <c r="K44" s="39"/>
-      <c r="L44" s="39"/>
-      <c r="M44" s="39"/>
-      <c r="N44" s="39"/>
-      <c r="O44" s="40"/>
+      <c r="B44" s="102"/>
+      <c r="C44" s="103"/>
+      <c r="D44" s="104"/>
+      <c r="E44" s="95"/>
+      <c r="F44" s="93"/>
+      <c r="G44" s="93"/>
+      <c r="H44" s="93"/>
+      <c r="I44" s="93"/>
+      <c r="J44" s="93"/>
+      <c r="K44" s="93"/>
+      <c r="L44" s="93"/>
+      <c r="M44" s="93"/>
+      <c r="N44" s="93"/>
+      <c r="O44" s="94"/>
     </row>
     <row r="45" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B45" s="48"/>
-      <c r="C45" s="49"/>
-      <c r="D45" s="50"/>
-      <c r="E45" s="41"/>
-      <c r="F45" s="39"/>
-      <c r="G45" s="39"/>
-      <c r="H45" s="39"/>
-      <c r="I45" s="39"/>
-      <c r="J45" s="39"/>
-      <c r="K45" s="39"/>
-      <c r="L45" s="39"/>
-      <c r="M45" s="39"/>
-      <c r="N45" s="39"/>
-      <c r="O45" s="40"/>
+      <c r="B45" s="102"/>
+      <c r="C45" s="103"/>
+      <c r="D45" s="104"/>
+      <c r="E45" s="95"/>
+      <c r="F45" s="93"/>
+      <c r="G45" s="93"/>
+      <c r="H45" s="93"/>
+      <c r="I45" s="93"/>
+      <c r="J45" s="93"/>
+      <c r="K45" s="93"/>
+      <c r="L45" s="93"/>
+      <c r="M45" s="93"/>
+      <c r="N45" s="93"/>
+      <c r="O45" s="94"/>
     </row>
     <row r="46" spans="2:15" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B46" s="51"/>
-      <c r="C46" s="52"/>
-      <c r="D46" s="53"/>
-      <c r="E46" s="42"/>
-      <c r="F46" s="43"/>
-      <c r="G46" s="43"/>
-      <c r="H46" s="43"/>
-      <c r="I46" s="43"/>
-      <c r="J46" s="43"/>
-      <c r="K46" s="43"/>
-      <c r="L46" s="43"/>
-      <c r="M46" s="43"/>
-      <c r="N46" s="43"/>
-      <c r="O46" s="44"/>
+      <c r="B46" s="105"/>
+      <c r="C46" s="106"/>
+      <c r="D46" s="107"/>
+      <c r="E46" s="96"/>
+      <c r="F46" s="97"/>
+      <c r="G46" s="97"/>
+      <c r="H46" s="97"/>
+      <c r="I46" s="97"/>
+      <c r="J46" s="97"/>
+      <c r="K46" s="97"/>
+      <c r="L46" s="97"/>
+      <c r="M46" s="97"/>
+      <c r="N46" s="97"/>
+      <c r="O46" s="98"/>
     </row>
   </sheetData>
   <mergeCells count="43">
-    <mergeCell ref="B17:D17"/>
-    <mergeCell ref="J6:K6"/>
-    <mergeCell ref="L6:O6"/>
-    <mergeCell ref="E6:I6"/>
-    <mergeCell ref="E17:F17"/>
-    <mergeCell ref="G17:H17"/>
-    <mergeCell ref="B13:H13"/>
-    <mergeCell ref="B14:D14"/>
-    <mergeCell ref="B15:D15"/>
-    <mergeCell ref="B16:D16"/>
-    <mergeCell ref="E9:G9"/>
-    <mergeCell ref="B8:D9"/>
-    <mergeCell ref="B19:F19"/>
-    <mergeCell ref="B11:O11"/>
-    <mergeCell ref="K25:O26"/>
-    <mergeCell ref="H9:O9"/>
-    <mergeCell ref="J20:O20"/>
-    <mergeCell ref="B22:O22"/>
-    <mergeCell ref="B24:I24"/>
-    <mergeCell ref="K24:O24"/>
-    <mergeCell ref="E18:F18"/>
-    <mergeCell ref="G19:H19"/>
-    <mergeCell ref="E15:F15"/>
-    <mergeCell ref="E16:F16"/>
-    <mergeCell ref="G15:H15"/>
-    <mergeCell ref="G16:H16"/>
-    <mergeCell ref="G18:H18"/>
     <mergeCell ref="E40:O40"/>
     <mergeCell ref="E41:O46"/>
     <mergeCell ref="B40:D46"/>
@@ -2890,6 +2863,33 @@
     <mergeCell ref="B4:D4"/>
     <mergeCell ref="B5:D5"/>
     <mergeCell ref="B6:D6"/>
+    <mergeCell ref="B19:F19"/>
+    <mergeCell ref="B11:O11"/>
+    <mergeCell ref="K25:O26"/>
+    <mergeCell ref="H9:O9"/>
+    <mergeCell ref="J20:O20"/>
+    <mergeCell ref="B22:O22"/>
+    <mergeCell ref="B24:I24"/>
+    <mergeCell ref="K24:O24"/>
+    <mergeCell ref="E18:F18"/>
+    <mergeCell ref="G19:H19"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="G15:H15"/>
+    <mergeCell ref="G16:H16"/>
+    <mergeCell ref="G18:H18"/>
+    <mergeCell ref="B17:D17"/>
+    <mergeCell ref="J6:K6"/>
+    <mergeCell ref="L6:O6"/>
+    <mergeCell ref="E6:I6"/>
+    <mergeCell ref="E17:F17"/>
+    <mergeCell ref="G17:H17"/>
+    <mergeCell ref="B13:H13"/>
+    <mergeCell ref="B14:D14"/>
+    <mergeCell ref="B15:D15"/>
+    <mergeCell ref="B16:D16"/>
+    <mergeCell ref="E9:G9"/>
+    <mergeCell ref="B8:D9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="57" orientation="portrait" r:id="rId1"/>
@@ -2913,15 +2913,15 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B2" s="7">
         <v>4</v>
@@ -2929,7 +2929,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B3" s="7">
         <v>5</v>
@@ -2937,7 +2937,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B4" s="7">
         <v>2</v>
@@ -2945,7 +2945,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B5" s="7">
         <v>1</v>
@@ -2953,7 +2953,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B6" s="7">
         <v>3</v>
@@ -2961,7 +2961,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="16" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B7" s="16">
         <v>2</v>

</xml_diff>